<commit_message>
update Shiwang'Andu merging issue
</commit_message>
<xml_diff>
--- a/ZMB_admin_crosswalk.xlsx
+++ b/ZMB_admin_crosswalk.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38580" yWindow="1860" windowWidth="28160" windowHeight="15760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="620" yWindow="920" windowWidth="28160" windowHeight="15760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="number of constituencies" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="2016_renamed" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">crosswalk!$A$1:$J$178</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">crosswalk!$A$1:$J$157</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2467" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2467" uniqueCount="283">
   <si>
     <t>provinces</t>
   </si>
@@ -880,6 +880,9 @@
   </si>
   <si>
     <t>shp2015, shp2016</t>
+  </si>
+  <si>
+    <t>Shiwang'Andu</t>
   </si>
 </sst>
 </file>
@@ -1372,11 +1375,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C165" sqref="C165"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D158" sqref="D158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1418,7 +1422,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>212</v>
       </c>
@@ -1447,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>212</v>
       </c>
@@ -1476,7 +1480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>212</v>
       </c>
@@ -1505,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>212</v>
       </c>
@@ -1534,7 +1538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>212</v>
       </c>
@@ -1566,7 +1570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>212</v>
       </c>
@@ -1595,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>212</v>
       </c>
@@ -1624,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>212</v>
       </c>
@@ -1653,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>212</v>
       </c>
@@ -1682,7 +1686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>212</v>
       </c>
@@ -1711,7 +1715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>212</v>
       </c>
@@ -1740,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>212</v>
       </c>
@@ -1769,7 +1773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>212</v>
       </c>
@@ -1801,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>212</v>
       </c>
@@ -1830,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>212</v>
       </c>
@@ -1862,7 +1866,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>202</v>
       </c>
@@ -1891,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>202</v>
       </c>
@@ -1920,7 +1924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>202</v>
       </c>
@@ -1949,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>202</v>
       </c>
@@ -1978,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>202</v>
       </c>
@@ -2007,7 +2011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>202</v>
       </c>
@@ -2036,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>202</v>
       </c>
@@ -2065,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>202</v>
       </c>
@@ -2094,7 +2098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>202</v>
       </c>
@@ -2123,7 +2127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>202</v>
       </c>
@@ -2152,7 +2156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>202</v>
       </c>
@@ -2181,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>202</v>
       </c>
@@ -2210,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>202</v>
       </c>
@@ -2239,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>202</v>
       </c>
@@ -2268,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>202</v>
       </c>
@@ -2300,7 +2304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>202</v>
       </c>
@@ -2329,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>202</v>
       </c>
@@ -2358,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>202</v>
       </c>
@@ -2387,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>202</v>
       </c>
@@ -2419,7 +2423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>202</v>
       </c>
@@ -2448,7 +2452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>202</v>
       </c>
@@ -2477,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>202</v>
       </c>
@@ -2506,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>206</v>
       </c>
@@ -2535,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>206</v>
       </c>
@@ -2564,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>206</v>
       </c>
@@ -2593,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>206</v>
       </c>
@@ -2622,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>206</v>
       </c>
@@ -2651,7 +2655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>206</v>
       </c>
@@ -2680,7 +2684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>206</v>
       </c>
@@ -2709,7 +2713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>206</v>
       </c>
@@ -2738,7 +2742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>206</v>
       </c>
@@ -2767,7 +2771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>206</v>
       </c>
@@ -2796,7 +2800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>206</v>
       </c>
@@ -2825,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>206</v>
       </c>
@@ -2854,7 +2858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>206</v>
       </c>
@@ -2886,7 +2890,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>206</v>
       </c>
@@ -2915,7 +2919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>206</v>
       </c>
@@ -2944,7 +2948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>206</v>
       </c>
@@ -2976,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>206</v>
       </c>
@@ -3005,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>206</v>
       </c>
@@ -3034,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>150</v>
       </c>
@@ -3066,7 +3070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>150</v>
       </c>
@@ -3098,7 +3102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>150</v>
       </c>
@@ -3127,7 +3131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>150</v>
       </c>
@@ -3156,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>150</v>
       </c>
@@ -3185,7 +3189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>150</v>
       </c>
@@ -3214,7 +3218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>150</v>
       </c>
@@ -3243,7 +3247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>150</v>
       </c>
@@ -3272,7 +3276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>150</v>
       </c>
@@ -3304,7 +3308,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>150</v>
       </c>
@@ -3333,7 +3337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>150</v>
       </c>
@@ -3362,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>150</v>
       </c>
@@ -3391,7 +3395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>150</v>
       </c>
@@ -3420,7 +3424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>150</v>
       </c>
@@ -3449,7 +3453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>150</v>
       </c>
@@ -3478,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>220</v>
       </c>
@@ -3507,7 +3511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>220</v>
       </c>
@@ -3539,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>220</v>
       </c>
@@ -3568,7 +3572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>220</v>
       </c>
@@ -3597,7 +3601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>220</v>
       </c>
@@ -3626,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>220</v>
       </c>
@@ -3655,7 +3659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>220</v>
       </c>
@@ -3684,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>220</v>
       </c>
@@ -3713,7 +3717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>220</v>
       </c>
@@ -3742,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>220</v>
       </c>
@@ -3771,7 +3775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>220</v>
       </c>
@@ -3800,7 +3804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>220</v>
       </c>
@@ -3829,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>220</v>
       </c>
@@ -3858,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>220</v>
       </c>
@@ -4168,7 +4172,7 @@
         <v>172</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>94</v>
+        <v>282</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>172</v>
@@ -4189,7 +4193,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>199</v>
       </c>
@@ -4218,7 +4222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>199</v>
       </c>
@@ -4250,7 +4254,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>199</v>
       </c>
@@ -4282,7 +4286,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>199</v>
       </c>
@@ -4311,7 +4315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>199</v>
       </c>
@@ -4343,7 +4347,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>199</v>
       </c>
@@ -4372,7 +4376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>199</v>
       </c>
@@ -4404,7 +4408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>199</v>
       </c>
@@ -4433,7 +4437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>199</v>
       </c>
@@ -4462,7 +4466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>199</v>
       </c>
@@ -4491,7 +4495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>199</v>
       </c>
@@ -4520,7 +4524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>199</v>
       </c>
@@ -4549,7 +4553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>207</v>
       </c>
@@ -4578,7 +4582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>207</v>
       </c>
@@ -4607,7 +4611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>207</v>
       </c>
@@ -4636,7 +4640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>207</v>
       </c>
@@ -4665,7 +4669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>207</v>
       </c>
@@ -4694,7 +4698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>207</v>
       </c>
@@ -4723,7 +4727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>207</v>
       </c>
@@ -4752,7 +4756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>207</v>
       </c>
@@ -4781,7 +4785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>207</v>
       </c>
@@ -4810,7 +4814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>207</v>
       </c>
@@ -4839,7 +4843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>207</v>
       </c>
@@ -4868,7 +4872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>207</v>
       </c>
@@ -4897,7 +4901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>207</v>
       </c>
@@ -4926,7 +4930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>191</v>
       </c>
@@ -4955,7 +4959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>191</v>
       </c>
@@ -4984,7 +4988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>191</v>
       </c>
@@ -5013,7 +5017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>191</v>
       </c>
@@ -5042,7 +5046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>191</v>
       </c>
@@ -5071,7 +5075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>191</v>
       </c>
@@ -5100,7 +5104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>191</v>
       </c>
@@ -5129,7 +5133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>191</v>
       </c>
@@ -5158,7 +5162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>191</v>
       </c>
@@ -5187,7 +5191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>191</v>
       </c>
@@ -5216,7 +5220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>191</v>
       </c>
@@ -5245,7 +5249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>191</v>
       </c>
@@ -5274,7 +5278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>191</v>
       </c>
@@ -5303,7 +5307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>191</v>
       </c>
@@ -5332,7 +5336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>191</v>
       </c>
@@ -5361,7 +5365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>191</v>
       </c>
@@ -5390,7 +5394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>191</v>
       </c>
@@ -5419,7 +5423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>191</v>
       </c>
@@ -5448,7 +5452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>193</v>
       </c>
@@ -5477,7 +5481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>193</v>
       </c>
@@ -5506,7 +5510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>193</v>
       </c>
@@ -5535,7 +5539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>193</v>
       </c>
@@ -5564,7 +5568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>193</v>
       </c>
@@ -5593,7 +5597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>193</v>
       </c>
@@ -5622,7 +5626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>193</v>
       </c>
@@ -5651,7 +5655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>193</v>
       </c>
@@ -5683,7 +5687,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>193</v>
       </c>
@@ -5712,7 +5716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>193</v>
       </c>
@@ -5741,7 +5745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>193</v>
       </c>
@@ -5770,7 +5774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>193</v>
       </c>
@@ -5799,7 +5803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>193</v>
       </c>
@@ -5828,7 +5832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>193</v>
       </c>
@@ -5860,7 +5864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>193</v>
       </c>
@@ -5892,7 +5896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>193</v>
       </c>
@@ -5924,7 +5928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>193</v>
       </c>
@@ -5956,7 +5960,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>193</v>
       </c>
@@ -5985,7 +5989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>193</v>
       </c>
@@ -6228,6 +6232,13 @@
       <c r="H178" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J157">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Muchinga"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:J178">
     <sortCondition ref="A2:A178"/>
     <sortCondition ref="B2:B178"/>

</xml_diff>

<commit_message>
add in 2011 admin crosswalk
</commit_message>
<xml_diff>
--- a/ZMB_admin_crosswalk.xlsx
+++ b/ZMB_admin_crosswalk.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurahughes/Documents/GitHub/Zambia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laura/Documents/GitHub/Zambia/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,9 +23,6 @@
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2467" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2469" uniqueCount="285">
   <si>
     <t>provinces</t>
   </si>
@@ -883,6 +880,12 @@
   </si>
   <si>
     <t>Shiwang'Andu</t>
+  </si>
+  <si>
+    <t>website2011</t>
+  </si>
+  <si>
+    <t>Shiwang'andu</t>
   </si>
 </sst>
 </file>
@@ -1375,12 +1378,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J178"/>
+  <dimension ref="A1:K178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D158" sqref="D158"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K95" sqref="K95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1390,7 +1392,7 @@
     <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>188</v>
       </c>
@@ -1421,8 +1423,11 @@
       <c r="J1" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K1" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>212</v>
       </c>
@@ -1450,8 +1455,12 @@
       <c r="I2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K2" t="str">
+        <f>E2</f>
+        <v>Katuba</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>212</v>
       </c>
@@ -1479,8 +1488,12 @@
       <c r="I3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K66" si="0">E3</f>
+        <v>Keembe</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>212</v>
       </c>
@@ -1508,8 +1521,12 @@
       <c r="I4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>Chisamba</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>212</v>
       </c>
@@ -1537,8 +1554,12 @@
       <c r="I5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>Chitambo</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>212</v>
       </c>
@@ -1569,8 +1590,12 @@
       <c r="J6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>Itezhitezhi</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>212</v>
       </c>
@@ -1598,8 +1623,12 @@
       <c r="I7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>Bwacha</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>212</v>
       </c>
@@ -1627,8 +1656,12 @@
       <c r="I8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>Kabwe Central</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>212</v>
       </c>
@@ -1656,8 +1689,12 @@
       <c r="I9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>Kapiri Mposhi</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>212</v>
       </c>
@@ -1685,8 +1722,12 @@
       <c r="I10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>Mkushi South</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>212</v>
       </c>
@@ -1714,8 +1755,12 @@
       <c r="I11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>Mkushi North</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>212</v>
       </c>
@@ -1743,8 +1788,12 @@
       <c r="I12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>Mumbwa</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>212</v>
       </c>
@@ -1772,8 +1821,12 @@
       <c r="I13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>Nangoma</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>212</v>
       </c>
@@ -1804,8 +1857,12 @@
       <c r="J14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>212</v>
       </c>
@@ -1833,8 +1890,12 @@
       <c r="I15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>Muchinga</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>212</v>
       </c>
@@ -1865,8 +1926,12 @@
       <c r="J16" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>Serenje</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>202</v>
       </c>
@@ -1894,8 +1959,12 @@
       <c r="I17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>Chililabombwe</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>202</v>
       </c>
@@ -1923,8 +1992,12 @@
       <c r="I18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>Chingola</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>202</v>
       </c>
@@ -1952,8 +2025,12 @@
       <c r="I19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>Nchanga</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>202</v>
       </c>
@@ -1981,8 +2058,12 @@
       <c r="I20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v>Kalulushi</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>202</v>
       </c>
@@ -2010,8 +2091,12 @@
       <c r="I21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K21" t="str">
+        <f t="shared" si="0"/>
+        <v>Chimwemwe</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>202</v>
       </c>
@@ -2039,8 +2124,12 @@
       <c r="I22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K22" t="str">
+        <f t="shared" si="0"/>
+        <v>Kamfinsa</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>202</v>
       </c>
@@ -2068,8 +2157,12 @@
       <c r="I23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K23" t="str">
+        <f t="shared" si="0"/>
+        <v>Kwacha</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>202</v>
       </c>
@@ -2097,8 +2190,12 @@
       <c r="I24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K24" t="str">
+        <f t="shared" si="0"/>
+        <v>Nkana</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>202</v>
       </c>
@@ -2126,8 +2223,12 @@
       <c r="I25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K25" t="str">
+        <f t="shared" si="0"/>
+        <v>Wusakile</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>202</v>
       </c>
@@ -2155,8 +2256,12 @@
       <c r="I26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K26" t="str">
+        <f t="shared" si="0"/>
+        <v>Luanshya</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>202</v>
       </c>
@@ -2184,8 +2289,12 @@
       <c r="I27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K27" t="str">
+        <f t="shared" si="0"/>
+        <v>Roan</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>202</v>
       </c>
@@ -2213,8 +2322,12 @@
       <c r="I28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K28" t="str">
+        <f t="shared" si="0"/>
+        <v>Lufwanyama</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>202</v>
       </c>
@@ -2242,8 +2355,12 @@
       <c r="I29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K29" t="str">
+        <f t="shared" si="0"/>
+        <v>Kafulafuta</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>202</v>
       </c>
@@ -2271,8 +2388,12 @@
       <c r="I30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K30" t="str">
+        <f t="shared" si="0"/>
+        <v>Masaiti</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>202</v>
       </c>
@@ -2303,8 +2424,12 @@
       <c r="J31" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K31" t="str">
+        <f t="shared" si="0"/>
+        <v>Mpongwe</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>202</v>
       </c>
@@ -2332,8 +2457,12 @@
       <c r="I32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K32" t="str">
+        <f t="shared" si="0"/>
+        <v>Kankoyo</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>202</v>
       </c>
@@ -2361,8 +2490,12 @@
       <c r="I33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K33" t="str">
+        <f t="shared" si="0"/>
+        <v>Kantanshi</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>202</v>
       </c>
@@ -2390,8 +2523,12 @@
       <c r="I34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K34" t="str">
+        <f t="shared" si="0"/>
+        <v>Mufulira</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>202</v>
       </c>
@@ -2422,8 +2559,12 @@
       <c r="J35" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K35" t="str">
+        <f t="shared" si="0"/>
+        <v>Bwana Mkubwa</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>202</v>
       </c>
@@ -2451,8 +2592,12 @@
       <c r="I36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K36" t="str">
+        <f t="shared" si="0"/>
+        <v>Chifubu</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>202</v>
       </c>
@@ -2480,8 +2625,12 @@
       <c r="I37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K37" t="str">
+        <f t="shared" si="0"/>
+        <v>Kabushi</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>202</v>
       </c>
@@ -2509,8 +2658,12 @@
       <c r="I38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K38" t="str">
+        <f t="shared" si="0"/>
+        <v>Ndola Central</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>206</v>
       </c>
@@ -2538,8 +2691,12 @@
       <c r="I39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K39" t="str">
+        <f t="shared" si="0"/>
+        <v>Chadiza</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>206</v>
       </c>
@@ -2567,8 +2724,12 @@
       <c r="I40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K40" t="str">
+        <f t="shared" si="0"/>
+        <v>Chipangali</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>206</v>
       </c>
@@ -2596,8 +2757,12 @@
       <c r="I41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K41" t="str">
+        <f t="shared" si="0"/>
+        <v>Chipata Central</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>206</v>
       </c>
@@ -2625,8 +2790,12 @@
       <c r="I42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K42" t="str">
+        <f t="shared" si="0"/>
+        <v>Kasenengwa</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>206</v>
       </c>
@@ -2654,8 +2823,12 @@
       <c r="I43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K43" t="str">
+        <f t="shared" si="0"/>
+        <v>Luangeni</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>206</v>
       </c>
@@ -2683,8 +2856,12 @@
       <c r="I44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K44" t="str">
+        <f t="shared" si="0"/>
+        <v>Milanzi</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>206</v>
       </c>
@@ -2712,8 +2889,12 @@
       <c r="I45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K45" t="str">
+        <f t="shared" si="0"/>
+        <v>Mkaika</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>206</v>
       </c>
@@ -2741,8 +2922,12 @@
       <c r="I46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K46" t="str">
+        <f t="shared" si="0"/>
+        <v>Chasefu</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>206</v>
       </c>
@@ -2770,8 +2955,12 @@
       <c r="I47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K47" t="str">
+        <f t="shared" si="0"/>
+        <v>Lumezi</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>206</v>
       </c>
@@ -2799,8 +2988,12 @@
       <c r="I48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K48" t="str">
+        <f t="shared" si="0"/>
+        <v>Lundazi</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>206</v>
       </c>
@@ -2828,8 +3021,12 @@
       <c r="I49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K49" t="str">
+        <f t="shared" si="0"/>
+        <v>Malambo</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>206</v>
       </c>
@@ -2857,8 +3054,12 @@
       <c r="I50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K50" t="str">
+        <f t="shared" si="0"/>
+        <v>Nyimba</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>206</v>
       </c>
@@ -2889,8 +3090,12 @@
       <c r="J51" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K51" t="str">
+        <f t="shared" si="0"/>
+        <v>Kapoche</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>206</v>
       </c>
@@ -2918,8 +3123,12 @@
       <c r="I52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K52" t="str">
+        <f t="shared" si="0"/>
+        <v>Msanzala</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>206</v>
       </c>
@@ -2947,8 +3156,12 @@
       <c r="I53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K53" t="str">
+        <f t="shared" si="0"/>
+        <v>Petauke</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>206</v>
       </c>
@@ -2979,8 +3192,12 @@
       <c r="J54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K54" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>206</v>
       </c>
@@ -3008,8 +3225,12 @@
       <c r="I55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K55" t="str">
+        <f t="shared" si="0"/>
+        <v>Sinda</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>206</v>
       </c>
@@ -3037,8 +3258,12 @@
       <c r="I56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K56" t="str">
+        <f t="shared" si="0"/>
+        <v>Vubwi</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>150</v>
       </c>
@@ -3069,8 +3294,12 @@
       <c r="J57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K57" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>150</v>
       </c>
@@ -3101,8 +3330,12 @@
       <c r="J58" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K58" t="str">
+        <f t="shared" si="0"/>
+        <v>Chienge</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>150</v>
       </c>
@@ -3130,8 +3363,12 @@
       <c r="I59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K59" t="str">
+        <f t="shared" si="0"/>
+        <v>Chipili</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>150</v>
       </c>
@@ -3159,8 +3396,12 @@
       <c r="I60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K60" t="str">
+        <f t="shared" si="0"/>
+        <v>Kawambwa</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>150</v>
       </c>
@@ -3188,8 +3429,12 @@
       <c r="I61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K61" t="str">
+        <f t="shared" si="0"/>
+        <v>Pambashe</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>150</v>
       </c>
@@ -3217,8 +3462,12 @@
       <c r="I62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K62" t="str">
+        <f t="shared" si="0"/>
+        <v>Luapula</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>150</v>
       </c>
@@ -3246,8 +3495,12 @@
       <c r="I63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K63" t="str">
+        <f t="shared" si="0"/>
+        <v>Bahati</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>150</v>
       </c>
@@ -3275,8 +3528,12 @@
       <c r="I64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K64" t="str">
+        <f t="shared" si="0"/>
+        <v>Mansa Central</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>150</v>
       </c>
@@ -3307,8 +3564,12 @@
       <c r="J65" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K65" t="str">
+        <f t="shared" si="0"/>
+        <v>Chembe</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>150</v>
       </c>
@@ -3336,8 +3597,12 @@
       <c r="I66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K66" t="str">
+        <f t="shared" si="0"/>
+        <v>Mwansabombwe</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>150</v>
       </c>
@@ -3365,8 +3630,12 @@
       <c r="I67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K67" t="str">
+        <f t="shared" ref="K67:K130" si="1">E67</f>
+        <v>Mambilima</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>150</v>
       </c>
@@ -3394,8 +3663,12 @@
       <c r="I68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K68" t="str">
+        <f t="shared" si="1"/>
+        <v>Mwense</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>150</v>
       </c>
@@ -3423,8 +3696,12 @@
       <c r="I69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K69" t="str">
+        <f t="shared" si="1"/>
+        <v>Nchelenge</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>150</v>
       </c>
@@ -3452,8 +3729,12 @@
       <c r="I70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K70" t="str">
+        <f t="shared" si="1"/>
+        <v>Bangweulu</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>150</v>
       </c>
@@ -3481,8 +3762,12 @@
       <c r="I71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K71" t="str">
+        <f t="shared" si="1"/>
+        <v>Chifunabuli</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>220</v>
       </c>
@@ -3510,8 +3795,12 @@
       <c r="I72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K72" t="str">
+        <f t="shared" si="1"/>
+        <v>Chilanga</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>220</v>
       </c>
@@ -3542,8 +3831,12 @@
       <c r="J73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K73" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>220</v>
       </c>
@@ -3571,8 +3864,12 @@
       <c r="I74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K74" t="str">
+        <f t="shared" si="1"/>
+        <v>Chongwe</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>220</v>
       </c>
@@ -3600,8 +3897,12 @@
       <c r="I75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K75" t="str">
+        <f t="shared" si="1"/>
+        <v>Kafue</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>220</v>
       </c>
@@ -3629,8 +3930,12 @@
       <c r="I76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K76" t="str">
+        <f t="shared" si="1"/>
+        <v>Feira</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>220</v>
       </c>
@@ -3658,8 +3963,12 @@
       <c r="I77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K77" t="str">
+        <f t="shared" si="1"/>
+        <v>Chawama</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>220</v>
       </c>
@@ -3687,8 +3996,12 @@
       <c r="I78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K78" t="str">
+        <f t="shared" si="1"/>
+        <v>Kabwata</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>220</v>
       </c>
@@ -3716,8 +4029,12 @@
       <c r="I79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K79" t="str">
+        <f t="shared" si="1"/>
+        <v>Kanyama</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>220</v>
       </c>
@@ -3745,8 +4062,12 @@
       <c r="I80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K80" t="str">
+        <f t="shared" si="1"/>
+        <v>Lusaka Central</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>220</v>
       </c>
@@ -3774,8 +4095,12 @@
       <c r="I81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K81" t="str">
+        <f t="shared" si="1"/>
+        <v>Mandevu</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>220</v>
       </c>
@@ -3803,8 +4128,12 @@
       <c r="I82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K82" t="str">
+        <f t="shared" si="1"/>
+        <v>Matero</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>220</v>
       </c>
@@ -3832,8 +4161,12 @@
       <c r="I83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K83" t="str">
+        <f t="shared" si="1"/>
+        <v>Munali</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>220</v>
       </c>
@@ -3861,8 +4194,12 @@
       <c r="I84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K84" t="str">
+        <f t="shared" si="1"/>
+        <v>Rufunsa</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>220</v>
       </c>
@@ -3890,8 +4227,12 @@
       <c r="I85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K85" t="str">
+        <f t="shared" si="1"/>
+        <v>Mwembezhi</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>119</v>
       </c>
@@ -3919,8 +4260,12 @@
       <c r="I86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K86" t="str">
+        <f t="shared" si="1"/>
+        <v>Chama North</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>119</v>
       </c>
@@ -3948,8 +4293,12 @@
       <c r="I87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K87" t="str">
+        <f t="shared" si="1"/>
+        <v>Chama South</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>119</v>
       </c>
@@ -3977,8 +4326,12 @@
       <c r="I88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K88" t="str">
+        <f t="shared" si="1"/>
+        <v>Chinsali</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>119</v>
       </c>
@@ -4009,8 +4362,12 @@
       <c r="J89" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K89" t="str">
+        <f t="shared" si="1"/>
+        <v>Isoka</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>119</v>
       </c>
@@ -4041,8 +4398,12 @@
       <c r="J90" s="2" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K90" t="str">
+        <f t="shared" si="1"/>
+        <v>Mafinga</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>119</v>
       </c>
@@ -4070,8 +4431,12 @@
       <c r="I91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K91" t="str">
+        <f t="shared" si="1"/>
+        <v>Kanchibiya</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>119</v>
       </c>
@@ -4099,8 +4464,12 @@
       <c r="I92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K92" t="str">
+        <f t="shared" si="1"/>
+        <v>Mfuwe</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>119</v>
       </c>
@@ -4131,8 +4500,12 @@
       <c r="J93" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K93" t="str">
+        <f t="shared" si="1"/>
+        <v>Mpika</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>119</v>
       </c>
@@ -4160,8 +4533,12 @@
       <c r="I94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K94" t="str">
+        <f t="shared" si="1"/>
+        <v>Nakonde</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>119</v>
       </c>
@@ -4192,8 +4569,11 @@
       <c r="J95" s="2" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K95" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>199</v>
       </c>
@@ -4221,8 +4601,12 @@
       <c r="I96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K96" t="str">
+        <f t="shared" si="1"/>
+        <v>Chavuma</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>199</v>
       </c>
@@ -4253,8 +4637,12 @@
       <c r="J97" s="2" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K97" t="str">
+        <f t="shared" si="1"/>
+        <v>Ikeleng'i</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>199</v>
       </c>
@@ -4285,8 +4673,12 @@
       <c r="J98" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K98" t="str">
+        <f t="shared" si="1"/>
+        <v>Kabompo West</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>199</v>
       </c>
@@ -4314,8 +4706,12 @@
       <c r="I99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K99" t="str">
+        <f t="shared" si="1"/>
+        <v>Kasempa</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>199</v>
       </c>
@@ -4346,8 +4742,12 @@
       <c r="J100" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K100" t="str">
+        <f t="shared" si="1"/>
+        <v>Kabompo East</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>199</v>
       </c>
@@ -4375,8 +4775,12 @@
       <c r="I101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K101" t="str">
+        <f t="shared" si="1"/>
+        <v>Mufumbwe</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>199</v>
       </c>
@@ -4407,8 +4811,12 @@
       <c r="J102" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K102" t="str">
+        <f t="shared" si="1"/>
+        <v>Mwinilunga</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>199</v>
       </c>
@@ -4436,8 +4844,12 @@
       <c r="I103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K103" t="str">
+        <f t="shared" si="1"/>
+        <v>Solwezi Central</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>199</v>
       </c>
@@ -4465,8 +4877,12 @@
       <c r="I104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K104" t="str">
+        <f t="shared" si="1"/>
+        <v>Solwezi East</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>199</v>
       </c>
@@ -4494,8 +4910,12 @@
       <c r="I105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K105" t="str">
+        <f t="shared" si="1"/>
+        <v>Solwezi West</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>199</v>
       </c>
@@ -4523,8 +4943,12 @@
       <c r="I106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K106" t="str">
+        <f t="shared" si="1"/>
+        <v>Zambezi East</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>199</v>
       </c>
@@ -4552,8 +4976,12 @@
       <c r="I107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K107" t="str">
+        <f t="shared" si="1"/>
+        <v>Zambezi West</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>207</v>
       </c>
@@ -4581,8 +5009,12 @@
       <c r="I108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K108" t="str">
+        <f t="shared" si="1"/>
+        <v>Chilubi</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>207</v>
       </c>
@@ -4610,8 +5042,12 @@
       <c r="I109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K109" t="str">
+        <f t="shared" si="1"/>
+        <v>Kaputa</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>207</v>
       </c>
@@ -4639,8 +5075,12 @@
       <c r="I110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K110" t="str">
+        <f t="shared" si="1"/>
+        <v>Kasama Central</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>207</v>
       </c>
@@ -4668,8 +5108,12 @@
       <c r="I111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K111" t="str">
+        <f t="shared" si="1"/>
+        <v>Lukashya</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>207</v>
       </c>
@@ -4697,8 +5141,12 @@
       <c r="I112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K112" t="str">
+        <f t="shared" si="1"/>
+        <v>Lubansenshi</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>207</v>
       </c>
@@ -4726,8 +5174,12 @@
       <c r="I113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K113" t="str">
+        <f t="shared" si="1"/>
+        <v>Lupososhi</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>207</v>
       </c>
@@ -4755,8 +5207,12 @@
       <c r="I114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K114" t="str">
+        <f t="shared" si="1"/>
+        <v>Mbala</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>207</v>
       </c>
@@ -4784,8 +5240,12 @@
       <c r="I115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K115" t="str">
+        <f t="shared" si="1"/>
+        <v>Senga Hill</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>207</v>
       </c>
@@ -4813,8 +5273,12 @@
       <c r="I116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K116" t="str">
+        <f t="shared" si="1"/>
+        <v>Lunte</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>207</v>
       </c>
@@ -4842,8 +5306,12 @@
       <c r="I117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K117" t="str">
+        <f t="shared" si="1"/>
+        <v>Mporokoso</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>207</v>
       </c>
@@ -4871,8 +5339,12 @@
       <c r="I118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K118" t="str">
+        <f t="shared" si="1"/>
+        <v>Mpulungu</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>207</v>
       </c>
@@ -4900,8 +5372,12 @@
       <c r="I119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K119" t="str">
+        <f t="shared" si="1"/>
+        <v>Malole</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>207</v>
       </c>
@@ -4929,8 +5405,12 @@
       <c r="I120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K120" t="str">
+        <f t="shared" si="1"/>
+        <v>Chimbamilonga</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>191</v>
       </c>
@@ -4958,8 +5438,12 @@
       <c r="I121">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K121" t="str">
+        <f t="shared" si="1"/>
+        <v>Chikankata</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>191</v>
       </c>
@@ -4987,8 +5471,12 @@
       <c r="I122">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K122" t="str">
+        <f t="shared" si="1"/>
+        <v>Choma Central</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>191</v>
       </c>
@@ -5016,8 +5504,12 @@
       <c r="I123">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K123" t="str">
+        <f t="shared" si="1"/>
+        <v>Mbabala</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>191</v>
       </c>
@@ -5045,8 +5537,12 @@
       <c r="I124">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K124" t="str">
+        <f t="shared" si="1"/>
+        <v>Gwembe</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>191</v>
       </c>
@@ -5074,8 +5570,12 @@
       <c r="I125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K125" t="str">
+        <f t="shared" si="1"/>
+        <v>Dundumwezi</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>191</v>
       </c>
@@ -5103,8 +5603,12 @@
       <c r="I126">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K126" t="str">
+        <f t="shared" si="1"/>
+        <v>Kalomo Central</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>191</v>
       </c>
@@ -5132,8 +5636,12 @@
       <c r="I127">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K127" t="str">
+        <f t="shared" si="1"/>
+        <v>Katombola</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>191</v>
       </c>
@@ -5161,8 +5669,12 @@
       <c r="I128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K128" t="str">
+        <f t="shared" si="1"/>
+        <v>Livingstone</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>191</v>
       </c>
@@ -5190,8 +5702,12 @@
       <c r="I129">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K129" t="str">
+        <f t="shared" si="1"/>
+        <v>Magoye</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>191</v>
       </c>
@@ -5219,8 +5735,12 @@
       <c r="I130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K130" t="str">
+        <f t="shared" si="1"/>
+        <v>Mazabuka Central</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>191</v>
       </c>
@@ -5248,8 +5768,12 @@
       <c r="I131">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K131" t="str">
+        <f t="shared" ref="K131:K157" si="2">E131</f>
+        <v>Bweengwa</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>191</v>
       </c>
@@ -5277,8 +5801,12 @@
       <c r="I132">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K132" t="str">
+        <f t="shared" si="2"/>
+        <v>Monze Central</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>191</v>
       </c>
@@ -5306,8 +5834,12 @@
       <c r="I133">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K133" t="str">
+        <f t="shared" si="2"/>
+        <v>Moomba</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>191</v>
       </c>
@@ -5335,8 +5867,12 @@
       <c r="I134">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K134" t="str">
+        <f t="shared" si="2"/>
+        <v>Namwala</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>191</v>
       </c>
@@ -5364,8 +5900,12 @@
       <c r="I135">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K135" t="str">
+        <f t="shared" si="2"/>
+        <v>Pemba</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>191</v>
       </c>
@@ -5393,8 +5933,12 @@
       <c r="I136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K136" t="str">
+        <f t="shared" si="2"/>
+        <v>Siavonga</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>191</v>
       </c>
@@ -5422,8 +5966,12 @@
       <c r="I137">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K137" t="str">
+        <f t="shared" si="2"/>
+        <v>Sinazongwe</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>191</v>
       </c>
@@ -5451,8 +5999,12 @@
       <c r="I138">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K138" t="str">
+        <f t="shared" si="2"/>
+        <v>Mapatizya</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>193</v>
       </c>
@@ -5480,8 +6032,12 @@
       <c r="I139">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K139" t="str">
+        <f t="shared" si="2"/>
+        <v>Kalabo Central</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>193</v>
       </c>
@@ -5509,8 +6065,12 @@
       <c r="I140">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K140" t="str">
+        <f t="shared" si="2"/>
+        <v>Liuwa</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>193</v>
       </c>
@@ -5538,8 +6098,12 @@
       <c r="I141">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K141" t="str">
+        <f t="shared" si="2"/>
+        <v>Kaoma Central</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>193</v>
       </c>
@@ -5567,8 +6131,12 @@
       <c r="I142">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K142" t="str">
+        <f t="shared" si="2"/>
+        <v>Mangango</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>193</v>
       </c>
@@ -5596,8 +6164,12 @@
       <c r="I143">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K143" t="str">
+        <f t="shared" si="2"/>
+        <v>Luena</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>193</v>
       </c>
@@ -5625,8 +6197,12 @@
       <c r="I144">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K144" t="str">
+        <f t="shared" si="2"/>
+        <v>Luampa</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>193</v>
       </c>
@@ -5654,8 +6230,12 @@
       <c r="I145">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K145" t="str">
+        <f t="shared" si="2"/>
+        <v>Lukulu East</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>193</v>
       </c>
@@ -5686,8 +6266,12 @@
       <c r="J146" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K146" t="str">
+        <f t="shared" si="2"/>
+        <v>Lukulu West</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>193</v>
       </c>
@@ -5715,8 +6299,12 @@
       <c r="I147">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K147" t="str">
+        <f t="shared" si="2"/>
+        <v>Mongu Central</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>193</v>
       </c>
@@ -5744,8 +6332,12 @@
       <c r="I148">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K148" t="str">
+        <f t="shared" si="2"/>
+        <v>Nalikwanda</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>193</v>
       </c>
@@ -5773,8 +6365,12 @@
       <c r="I149">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K149" t="str">
+        <f t="shared" si="2"/>
+        <v>Mulobezi</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>193</v>
       </c>
@@ -5802,8 +6398,12 @@
       <c r="I150">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K150" t="str">
+        <f t="shared" si="2"/>
+        <v>Mwandi</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>193</v>
       </c>
@@ -5831,8 +6431,12 @@
       <c r="I151">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K151" t="str">
+        <f t="shared" si="2"/>
+        <v>Nalolo</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>193</v>
       </c>
@@ -5863,8 +6467,12 @@
       <c r="J152">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K152" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>193</v>
       </c>
@@ -5895,8 +6503,12 @@
       <c r="J153" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K153" t="str">
+        <f t="shared" si="2"/>
+        <v>Senanga</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>193</v>
       </c>
@@ -5927,8 +6539,12 @@
       <c r="J154" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K154" t="str">
+        <f t="shared" si="2"/>
+        <v>Sesheke</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>193</v>
       </c>
@@ -5959,8 +6575,12 @@
       <c r="J155" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K155" t="str">
+        <f t="shared" si="2"/>
+        <v>Sinjembela</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>193</v>
       </c>
@@ -5988,8 +6608,12 @@
       <c r="I156">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K156" t="str">
+        <f t="shared" si="2"/>
+        <v>Sikongo</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>193</v>
       </c>
@@ -6020,8 +6644,12 @@
       <c r="J157">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K157" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -6031,7 +6659,7 @@
       <c r="G158" s="2"/>
       <c r="H158" s="2"/>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -6041,7 +6669,7 @@
       <c r="G159" s="2"/>
       <c r="H159" s="2"/>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -6232,13 +6860,6 @@
       <c r="H178" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J157">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Muchinga"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <sortState ref="A2:J178">
     <sortCondition ref="A2:A178"/>
     <sortCondition ref="B2:B178"/>

</xml_diff>

<commit_message>
fix 2008 merge error
</commit_message>
<xml_diff>
--- a/ZMB_admin_crosswalk.xlsx
+++ b/ZMB_admin_crosswalk.xlsx
@@ -1474,8 +1474,8 @@
   <dimension ref="A1:P178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O27" sqref="O27"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2:P156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5991,7 +5991,7 @@
         <v>79</v>
       </c>
       <c r="P93" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.2">
@@ -9320,11 +9320,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T177"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9394,7 +9393,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9455,7 +9454,7 @@
         <v>Katuba</v>
       </c>
     </row>
-    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9516,7 +9515,7 @@
         <v>Keembe</v>
       </c>
     </row>
-    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9577,7 +9576,7 @@
         <v>Chisamba</v>
       </c>
     </row>
-    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9638,7 +9637,7 @@
         <v>Chitambo</v>
       </c>
     </row>
-    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9702,7 +9701,7 @@
         <v>Itezhitezhi</v>
       </c>
     </row>
-    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -9763,7 +9762,7 @@
         <v>Bwacha</v>
       </c>
     </row>
-    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -9824,7 +9823,7 @@
         <v>Kabwe Central</v>
       </c>
     </row>
-    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -9885,7 +9884,7 @@
         <v>Kapiri Mposhi</v>
       </c>
     </row>
-    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -9946,7 +9945,7 @@
         <v>Mkushi South</v>
       </c>
     </row>
-    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -10007,7 +10006,7 @@
         <v>Mkushi North</v>
       </c>
     </row>
-    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -10068,7 +10067,7 @@
         <v>Mumbwa</v>
       </c>
     </row>
-    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -10129,7 +10128,7 @@
         <v>Nangoma</v>
       </c>
     </row>
-    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10190,7 +10189,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10315,7 +10314,7 @@
         <v>Serenje</v>
       </c>
     </row>
-    <row r="17" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -10376,7 +10375,7 @@
         <v>Chililabombwe</v>
       </c>
     </row>
-    <row r="18" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -10437,7 +10436,7 @@
         <v>Chingola</v>
       </c>
     </row>
-    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -10498,7 +10497,7 @@
         <v>Nchanga</v>
       </c>
     </row>
-    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -10559,7 +10558,7 @@
         <v>Kalulushi</v>
       </c>
     </row>
-    <row r="21" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -10620,7 +10619,7 @@
         <v>Chimwemwe</v>
       </c>
     </row>
-    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -10681,7 +10680,7 @@
         <v>Kamfinsa</v>
       </c>
     </row>
-    <row r="23" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -10742,7 +10741,7 @@
         <v>Kwacha</v>
       </c>
     </row>
-    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -10803,7 +10802,7 @@
         <v>Nkana</v>
       </c>
     </row>
-    <row r="25" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -10864,7 +10863,7 @@
         <v>Wusakile</v>
       </c>
     </row>
-    <row r="26" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -10925,7 +10924,7 @@
         <v>Luanshya</v>
       </c>
     </row>
-    <row r="27" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -10986,7 +10985,7 @@
         <v>Roan</v>
       </c>
     </row>
-    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -11047,7 +11046,7 @@
         <v>Lufwanyama</v>
       </c>
     </row>
-    <row r="29" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -11108,7 +11107,7 @@
         <v>Kafulafuta</v>
       </c>
     </row>
-    <row r="30" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -11169,7 +11168,7 @@
         <v>Masaiti</v>
       </c>
     </row>
-    <row r="31" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -11230,7 +11229,7 @@
         <v>Mpongwe</v>
       </c>
     </row>
-    <row r="32" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -11291,7 +11290,7 @@
         <v>Kankoyo</v>
       </c>
     </row>
-    <row r="33" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -11352,7 +11351,7 @@
         <v>Kantanshi</v>
       </c>
     </row>
-    <row r="34" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -11413,7 +11412,7 @@
         <v>Mufulira</v>
       </c>
     </row>
-    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -11477,7 +11476,7 @@
         <v>Bwanankubwa</v>
       </c>
     </row>
-    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -11538,7 +11537,7 @@
         <v>Chifubu</v>
       </c>
     </row>
-    <row r="37" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -11599,7 +11598,7 @@
         <v>Kabushi</v>
       </c>
     </row>
-    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -11660,7 +11659,7 @@
         <v>Ndola Central</v>
       </c>
     </row>
-    <row r="39" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -11721,7 +11720,7 @@
         <v>Chadiza</v>
       </c>
     </row>
-    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -11782,7 +11781,7 @@
         <v>Chipangali</v>
       </c>
     </row>
-    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -11843,7 +11842,7 @@
         <v>Chipata Central</v>
       </c>
     </row>
-    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -11904,7 +11903,7 @@
         <v>Kasenengwa</v>
       </c>
     </row>
-    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -11965,7 +11964,7 @@
         <v>Luangeni</v>
       </c>
     </row>
-    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -12026,7 +12025,7 @@
         <v>Milanzi</v>
       </c>
     </row>
-    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -12087,7 +12086,7 @@
         <v>Mkaika</v>
       </c>
     </row>
-    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -12148,7 +12147,7 @@
         <v>Chasefu</v>
       </c>
     </row>
-    <row r="47" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -12209,7 +12208,7 @@
         <v>Lumezi</v>
       </c>
     </row>
-    <row r="48" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -12270,7 +12269,7 @@
         <v>Lundazi</v>
       </c>
     </row>
-    <row r="49" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -12331,7 +12330,7 @@
         <v>Malambo</v>
       </c>
     </row>
-    <row r="50" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -12392,7 +12391,7 @@
         <v>Nyimba</v>
       </c>
     </row>
-    <row r="51" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -12453,7 +12452,7 @@
         <v>Kapoche</v>
       </c>
     </row>
-    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -12514,7 +12513,7 @@
         <v>Msanzala</v>
       </c>
     </row>
-    <row r="53" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -12575,7 +12574,7 @@
         <v>Petauke</v>
       </c>
     </row>
-    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -12636,7 +12635,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -12697,7 +12696,7 @@
         <v>Sinda</v>
       </c>
     </row>
-    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -12758,7 +12757,7 @@
         <v>Vubwi</v>
       </c>
     </row>
-    <row r="57" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -12819,7 +12818,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="58" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -12883,7 +12882,7 @@
         <v>Chienge</v>
       </c>
     </row>
-    <row r="59" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -12944,7 +12943,7 @@
         <v>Chipili</v>
       </c>
     </row>
-    <row r="60" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -13005,7 +13004,7 @@
         <v>Kawambwa</v>
       </c>
     </row>
-    <row r="61" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -13066,7 +13065,7 @@
         <v>Pambashe</v>
       </c>
     </row>
-    <row r="62" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -13127,7 +13126,7 @@
         <v>Luapula</v>
       </c>
     </row>
-    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -13188,7 +13187,7 @@
         <v>Bahati</v>
       </c>
     </row>
-    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -13249,7 +13248,7 @@
         <v>Mansa Central</v>
       </c>
     </row>
-    <row r="65" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -13310,7 +13309,7 @@
         <v>Chembe</v>
       </c>
     </row>
-    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -13371,7 +13370,7 @@
         <v>Mwansabombwe</v>
       </c>
     </row>
-    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -13432,7 +13431,7 @@
         <v>Mambilima</v>
       </c>
     </row>
-    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -13493,7 +13492,7 @@
         <v>Mwense</v>
       </c>
     </row>
-    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -13554,7 +13553,7 @@
         <v>Nchelenge</v>
       </c>
     </row>
-    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -13615,7 +13614,7 @@
         <v>Bangweulu</v>
       </c>
     </row>
-    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -13676,7 +13675,7 @@
         <v>Chifunabuli</v>
       </c>
     </row>
-    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -13737,7 +13736,7 @@
         <v>Chilanga</v>
       </c>
     </row>
-    <row r="73" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -13798,7 +13797,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -13859,7 +13858,7 @@
         <v>Chongwe</v>
       </c>
     </row>
-    <row r="75" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -13920,7 +13919,7 @@
         <v>Kafue</v>
       </c>
     </row>
-    <row r="76" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -13981,7 +13980,7 @@
         <v>Feira</v>
       </c>
     </row>
-    <row r="77" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -14042,7 +14041,7 @@
         <v>Chawama</v>
       </c>
     </row>
-    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -14103,7 +14102,7 @@
         <v>Kabwata</v>
       </c>
     </row>
-    <row r="79" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -14164,7 +14163,7 @@
         <v>Kanyama</v>
       </c>
     </row>
-    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -14225,7 +14224,7 @@
         <v>Lusaka Central</v>
       </c>
     </row>
-    <row r="81" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -14286,7 +14285,7 @@
         <v>Mandevu</v>
       </c>
     </row>
-    <row r="82" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -14347,7 +14346,7 @@
         <v>Matero</v>
       </c>
     </row>
-    <row r="83" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -14408,7 +14407,7 @@
         <v>Munali</v>
       </c>
     </row>
-    <row r="84" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -14469,7 +14468,7 @@
         <v>Rufunsa</v>
       </c>
     </row>
-    <row r="85" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -14530,7 +14529,7 @@
         <v>Mwembezhi</v>
       </c>
     </row>
-    <row r="86" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -14594,7 +14593,7 @@
         <v>Chama North</v>
       </c>
     </row>
-    <row r="87" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -14655,7 +14654,7 @@
         <v>Chama South</v>
       </c>
     </row>
-    <row r="88" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -14716,7 +14715,7 @@
         <v>Chinsali</v>
       </c>
     </row>
-    <row r="89" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -14777,7 +14776,7 @@
         <v>Isoka West</v>
       </c>
     </row>
-    <row r="90" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -14838,7 +14837,7 @@
         <v>Isoka East</v>
       </c>
     </row>
-    <row r="91" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -14899,7 +14898,7 @@
         <v>Kanchibiya</v>
       </c>
     </row>
-    <row r="92" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -14960,7 +14959,7 @@
         <v>Mfuwe</v>
       </c>
     </row>
-    <row r="93" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -15017,14 +15016,14 @@
         <v>0</v>
       </c>
       <c r="S93" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="T93" t="str">
         <f t="shared" si="3"/>
-        <v>Sesheke</v>
-      </c>
-    </row>
-    <row r="94" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+        <v>Mpika</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -15085,7 +15084,7 @@
         <v>Nakonde</v>
       </c>
     </row>
-    <row r="95" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -15146,7 +15145,7 @@
         <v>Shiwang'andu</v>
       </c>
     </row>
-    <row r="96" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -15207,7 +15206,7 @@
         <v>Chavuma</v>
       </c>
     </row>
-    <row r="97" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -15268,7 +15267,7 @@
         <v>Mwinilunga West</v>
       </c>
     </row>
-    <row r="98" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -15329,7 +15328,7 @@
         <v>Kabompo West</v>
       </c>
     </row>
-    <row r="99" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -15390,7 +15389,7 @@
         <v>Kasempa</v>
       </c>
     </row>
-    <row r="100" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -15451,7 +15450,7 @@
         <v>Kabompo East</v>
       </c>
     </row>
-    <row r="101" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -15512,7 +15511,7 @@
         <v>Mufumbwe</v>
       </c>
     </row>
-    <row r="102" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -15573,7 +15572,7 @@
         <v>Mwinilunga East</v>
       </c>
     </row>
-    <row r="103" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -15634,7 +15633,7 @@
         <v>Solwezi Central</v>
       </c>
     </row>
-    <row r="104" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -15695,7 +15694,7 @@
         <v>Solwezi East</v>
       </c>
     </row>
-    <row r="105" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -15756,7 +15755,7 @@
         <v>Solwezi West</v>
       </c>
     </row>
-    <row r="106" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -15817,7 +15816,7 @@
         <v>Zambezi East</v>
       </c>
     </row>
-    <row r="107" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -15878,7 +15877,7 @@
         <v>Zambezi West</v>
       </c>
     </row>
-    <row r="108" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -15939,7 +15938,7 @@
         <v>Chilubi</v>
       </c>
     </row>
-    <row r="109" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -16000,7 +15999,7 @@
         <v>Kaputa</v>
       </c>
     </row>
-    <row r="110" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -16061,7 +16060,7 @@
         <v>Kasama Central</v>
       </c>
     </row>
-    <row r="111" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -16122,7 +16121,7 @@
         <v>Lukashya</v>
       </c>
     </row>
-    <row r="112" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -16183,7 +16182,7 @@
         <v>Lubansenshi</v>
       </c>
     </row>
-    <row r="113" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -16244,7 +16243,7 @@
         <v>Lupososhi</v>
       </c>
     </row>
-    <row r="114" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -16305,7 +16304,7 @@
         <v>Mbala</v>
       </c>
     </row>
-    <row r="115" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -16366,7 +16365,7 @@
         <v>Senga Hill</v>
       </c>
     </row>
-    <row r="116" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -16427,7 +16426,7 @@
         <v>Lunte</v>
       </c>
     </row>
-    <row r="117" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -16488,7 +16487,7 @@
         <v>Mporokoso</v>
       </c>
     </row>
-    <row r="118" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -16549,7 +16548,7 @@
         <v>Mpulungu</v>
       </c>
     </row>
-    <row r="119" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -16610,7 +16609,7 @@
         <v>Malole</v>
       </c>
     </row>
-    <row r="120" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -16671,7 +16670,7 @@
         <v>Chimbamilonga</v>
       </c>
     </row>
-    <row r="121" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -16732,7 +16731,7 @@
         <v>Chikankata</v>
       </c>
     </row>
-    <row r="122" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -16793,7 +16792,7 @@
         <v>Choma Central</v>
       </c>
     </row>
-    <row r="123" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -16854,7 +16853,7 @@
         <v>Mbabala</v>
       </c>
     </row>
-    <row r="124" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -16915,7 +16914,7 @@
         <v>Gwembe</v>
       </c>
     </row>
-    <row r="125" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -16976,7 +16975,7 @@
         <v>Dundumwezi</v>
       </c>
     </row>
-    <row r="126" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -17037,7 +17036,7 @@
         <v>Kalomo Central</v>
       </c>
     </row>
-    <row r="127" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -17098,7 +17097,7 @@
         <v>Katombola</v>
       </c>
     </row>
-    <row r="128" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -17159,7 +17158,7 @@
         <v>Livingstone</v>
       </c>
     </row>
-    <row r="129" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -17220,7 +17219,7 @@
         <v>Magoye</v>
       </c>
     </row>
-    <row r="130" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -17281,7 +17280,7 @@
         <v>Mazabuka Central</v>
       </c>
     </row>
-    <row r="131" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -17342,7 +17341,7 @@
         <v>Bweengwa</v>
       </c>
     </row>
-    <row r="132" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -17403,7 +17402,7 @@
         <v>Monze Central</v>
       </c>
     </row>
-    <row r="133" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -17464,7 +17463,7 @@
         <v>Moomba</v>
       </c>
     </row>
-    <row r="134" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -17525,7 +17524,7 @@
         <v>Namwala</v>
       </c>
     </row>
-    <row r="135" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -17586,7 +17585,7 @@
         <v>Pemba</v>
       </c>
     </row>
-    <row r="136" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -17647,7 +17646,7 @@
         <v>Siavonga</v>
       </c>
     </row>
-    <row r="137" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -17708,7 +17707,7 @@
         <v>Sinazongwe</v>
       </c>
     </row>
-    <row r="138" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -17769,7 +17768,7 @@
         <v>Mapatizya</v>
       </c>
     </row>
-    <row r="139" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -17830,7 +17829,7 @@
         <v>Kalabo Central</v>
       </c>
     </row>
-    <row r="140" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -17891,7 +17890,7 @@
         <v>Liuwa</v>
       </c>
     </row>
-    <row r="141" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -17952,7 +17951,7 @@
         <v>Kaoma Central</v>
       </c>
     </row>
-    <row r="142" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -18013,7 +18012,7 @@
         <v>Mangango</v>
       </c>
     </row>
-    <row r="143" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -18074,7 +18073,7 @@
         <v>Luena</v>
       </c>
     </row>
-    <row r="144" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -18135,7 +18134,7 @@
         <v>Luampa</v>
       </c>
     </row>
-    <row r="145" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -18196,7 +18195,7 @@
         <v>Lukulu East</v>
       </c>
     </row>
-    <row r="146" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -18257,7 +18256,7 @@
         <v>Lukulu West</v>
       </c>
     </row>
-    <row r="147" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -18318,7 +18317,7 @@
         <v>Mongu Central</v>
       </c>
     </row>
-    <row r="148" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -18379,7 +18378,7 @@
         <v>Nalikwanda</v>
       </c>
     </row>
-    <row r="149" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -18440,7 +18439,7 @@
         <v>Mulobezi</v>
       </c>
     </row>
-    <row r="150" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -18501,7 +18500,7 @@
         <v>Mwandi</v>
       </c>
     </row>
-    <row r="151" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -18562,7 +18561,7 @@
         <v>Nalolo</v>
       </c>
     </row>
-    <row r="152" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -18623,7 +18622,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="153" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -18687,7 +18686,7 @@
         <v>Senanga</v>
       </c>
     </row>
-    <row r="154" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -18751,7 +18750,7 @@
         <v>Sesheke</v>
       </c>
     </row>
-    <row r="155" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -18812,7 +18811,7 @@
         <v>Sinjembela</v>
       </c>
     </row>
-    <row r="156" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
@@ -18873,7 +18872,7 @@
         <v>Sikongo</v>
       </c>
     </row>
-    <row r="157" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -18930,7 +18929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>16</v>
       </c>
@@ -18987,7 +18986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>16</v>
       </c>
@@ -19044,7 +19043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>16</v>
       </c>
@@ -19101,7 +19100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>16</v>
       </c>
@@ -19158,7 +19157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>16</v>
       </c>
@@ -19215,7 +19214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>16</v>
       </c>
@@ -19272,7 +19271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>16</v>
       </c>
@@ -19329,7 +19328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>16</v>
       </c>
@@ -19386,7 +19385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>16</v>
       </c>
@@ -19443,7 +19442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>16</v>
       </c>
@@ -19500,7 +19499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>16</v>
       </c>
@@ -19557,7 +19556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>16</v>
       </c>
@@ -19614,7 +19613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>16</v>
       </c>
@@ -19671,7 +19670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>16</v>
       </c>
@@ -19728,7 +19727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>16</v>
       </c>
@@ -19842,7 +19841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>16</v>
       </c>
@@ -19899,7 +19898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>16</v>
       </c>
@@ -19956,7 +19955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>16</v>
       </c>
@@ -20013,7 +20012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>16</v>
       </c>
@@ -20069,20 +20068,9 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T177">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R177">
-    <filterColumn colId="15">
-      <filters>
-        <filter val="Serenje"/>
-        <filter val="Serenje Central"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:R177"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
pull 2015 dists, merge
</commit_message>
<xml_diff>
--- a/ZMB_admin_crosswalk.xlsx
+++ b/ZMB_admin_crosswalk.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7899" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8217" uniqueCount="312">
   <si>
     <t>provinces</t>
   </si>
@@ -954,6 +954,24 @@
   <si>
     <t>fixed</t>
   </si>
+  <si>
+    <t>province2015</t>
+  </si>
+  <si>
+    <t>district2015</t>
+  </si>
+  <si>
+    <t>prov15_16</t>
+  </si>
+  <si>
+    <t>prov06_15</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Added Muchinga province</t>
+  </si>
 </sst>
 </file>
 
@@ -1351,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1363,7 +1381,7 @@
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1379,8 +1397,11 @@
       <c r="E1" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2017</v>
       </c>
@@ -1388,7 +1409,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2016</v>
       </c>
@@ -1405,10 +1426,16 @@
         <v>1571</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2015</v>
       </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>98</v>
+      </c>
       <c r="D4">
         <v>150</v>
       </c>
@@ -1416,7 +1443,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -1427,7 +1454,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2008</v>
       </c>
@@ -1435,15 +1462,24 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2006</v>
       </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>71</v>
+      </c>
       <c r="D7">
         <v>150</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2001</v>
       </c>
@@ -1451,7 +1487,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1996</v>
       </c>
@@ -1459,7 +1495,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1991</v>
       </c>
@@ -1471,11 +1507,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P178"/>
+  <dimension ref="A1:T178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2:P156"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1484,9 +1520,12 @@
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>289</v>
       </c>
@@ -1535,8 +1574,20 @@
       <c r="P1" s="1" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1583,8 +1634,22 @@
       <c r="P2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q2" t="s">
+        <v>212</v>
+      </c>
+      <c r="R2" t="s">
+        <v>222</v>
+      </c>
+      <c r="S2" t="b">
+        <f>Q2=B2</f>
+        <v>1</v>
+      </c>
+      <c r="T2" t="b">
+        <f>Q2=N2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1631,8 +1696,22 @@
       <c r="P3" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3" t="s">
+        <v>212</v>
+      </c>
+      <c r="R3" t="s">
+        <v>222</v>
+      </c>
+      <c r="S3" t="b">
+        <f t="shared" ref="S3:S66" si="1">Q3=B3</f>
+        <v>1</v>
+      </c>
+      <c r="T3" t="b">
+        <f t="shared" ref="T3:T66" si="2">Q3=N3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1679,8 +1758,22 @@
       <c r="P4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q4" t="s">
+        <v>212</v>
+      </c>
+      <c r="R4" t="s">
+        <v>123</v>
+      </c>
+      <c r="S4" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T4" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1727,8 +1820,22 @@
       <c r="P5" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5" t="s">
+        <v>212</v>
+      </c>
+      <c r="R5" t="s">
+        <v>118</v>
+      </c>
+      <c r="S5" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T5" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1778,8 +1885,22 @@
       <c r="P6" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q6" t="s">
+        <v>212</v>
+      </c>
+      <c r="R6" t="s">
+        <v>165</v>
+      </c>
+      <c r="S6" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T6" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1826,8 +1947,22 @@
       <c r="P7" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q7" t="s">
+        <v>212</v>
+      </c>
+      <c r="R7" t="s">
+        <v>219</v>
+      </c>
+      <c r="S7" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T7" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1874,8 +2009,22 @@
       <c r="P8" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q8" t="s">
+        <v>212</v>
+      </c>
+      <c r="R8" t="s">
+        <v>219</v>
+      </c>
+      <c r="S8" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T8" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1922,8 +2071,22 @@
       <c r="P9" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q9" t="s">
+        <v>212</v>
+      </c>
+      <c r="R9" t="s">
+        <v>95</v>
+      </c>
+      <c r="S9" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T9" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1970,8 +2133,22 @@
       <c r="P10" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q10" t="s">
+        <v>212</v>
+      </c>
+      <c r="R10" t="s">
+        <v>218</v>
+      </c>
+      <c r="S10" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T10" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2018,8 +2195,22 @@
       <c r="P11" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q11" t="s">
+        <v>212</v>
+      </c>
+      <c r="R11" t="s">
+        <v>217</v>
+      </c>
+      <c r="S11" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T11" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2066,8 +2257,22 @@
       <c r="P12" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q12" t="s">
+        <v>212</v>
+      </c>
+      <c r="R12" t="s">
+        <v>126</v>
+      </c>
+      <c r="S12" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T12" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2114,8 +2319,22 @@
       <c r="P13" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q13" t="s">
+        <v>212</v>
+      </c>
+      <c r="R13" t="s">
+        <v>126</v>
+      </c>
+      <c r="S13" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T13" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2165,8 +2384,22 @@
       <c r="P14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q14" t="s">
+        <v>16</v>
+      </c>
+      <c r="R14" t="s">
+        <v>16</v>
+      </c>
+      <c r="S14" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T14" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2213,8 +2446,22 @@
       <c r="P15" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q15" t="s">
+        <v>212</v>
+      </c>
+      <c r="R15" t="s">
+        <v>170</v>
+      </c>
+      <c r="S15" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T15" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2264,8 +2511,22 @@
       <c r="P16" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q16" t="s">
+        <v>212</v>
+      </c>
+      <c r="R16" t="s">
+        <v>170</v>
+      </c>
+      <c r="S16" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T16" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2312,8 +2573,22 @@
       <c r="P17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q17" t="s">
+        <v>202</v>
+      </c>
+      <c r="R17" t="s">
+        <v>49</v>
+      </c>
+      <c r="S17" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T17" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2360,8 +2635,22 @@
       <c r="P18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q18" t="s">
+        <v>202</v>
+      </c>
+      <c r="R18" t="s">
+        <v>50</v>
+      </c>
+      <c r="S18" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T18" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2408,8 +2697,22 @@
       <c r="P19" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q19" t="s">
+        <v>202</v>
+      </c>
+      <c r="R19" t="s">
+        <v>50</v>
+      </c>
+      <c r="S19" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T19" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2456,8 +2759,22 @@
       <c r="P20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q20" t="s">
+        <v>202</v>
+      </c>
+      <c r="R20" t="s">
+        <v>52</v>
+      </c>
+      <c r="S20" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T20" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2504,8 +2821,22 @@
       <c r="P21" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q21" t="s">
+        <v>202</v>
+      </c>
+      <c r="R21" t="s">
+        <v>204</v>
+      </c>
+      <c r="S21" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T21" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2552,8 +2883,22 @@
       <c r="P22" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q22" t="s">
+        <v>202</v>
+      </c>
+      <c r="R22" t="s">
+        <v>204</v>
+      </c>
+      <c r="S22" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T22" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2600,8 +2945,22 @@
       <c r="P23" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q23" t="s">
+        <v>202</v>
+      </c>
+      <c r="R23" t="s">
+        <v>204</v>
+      </c>
+      <c r="S23" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T23" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2648,8 +3007,22 @@
       <c r="P24" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q24" t="s">
+        <v>202</v>
+      </c>
+      <c r="R24" t="s">
+        <v>204</v>
+      </c>
+      <c r="S24" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T24" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2696,8 +3069,22 @@
       <c r="P25" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q25" t="s">
+        <v>202</v>
+      </c>
+      <c r="R25" t="s">
+        <v>204</v>
+      </c>
+      <c r="S25" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T25" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2744,8 +3131,22 @@
       <c r="P26" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q26" t="s">
+        <v>202</v>
+      </c>
+      <c r="R26" t="s">
+        <v>63</v>
+      </c>
+      <c r="S26" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T26" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2792,8 +3193,22 @@
       <c r="P27" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q27" t="s">
+        <v>202</v>
+      </c>
+      <c r="R27" t="s">
+        <v>63</v>
+      </c>
+      <c r="S27" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T27" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2840,8 +3255,22 @@
       <c r="P28" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q28" t="s">
+        <v>202</v>
+      </c>
+      <c r="R28" t="s">
+        <v>106</v>
+      </c>
+      <c r="S28" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T28" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2888,8 +3317,22 @@
       <c r="P29" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q29" t="s">
+        <v>202</v>
+      </c>
+      <c r="R29" t="s">
+        <v>47</v>
+      </c>
+      <c r="S29" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T29" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2936,8 +3379,22 @@
       <c r="P30" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q30" t="s">
+        <v>202</v>
+      </c>
+      <c r="R30" t="s">
+        <v>47</v>
+      </c>
+      <c r="S30" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T30" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2987,8 +3444,22 @@
       <c r="P31" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q31" t="s">
+        <v>202</v>
+      </c>
+      <c r="R31" t="s">
+        <v>45</v>
+      </c>
+      <c r="S31" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T31" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3035,8 +3506,22 @@
       <c r="P32" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q32" t="s">
+        <v>202</v>
+      </c>
+      <c r="R32" t="s">
+        <v>58</v>
+      </c>
+      <c r="S32" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T32" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3083,8 +3568,22 @@
       <c r="P33" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q33" t="s">
+        <v>202</v>
+      </c>
+      <c r="R33" t="s">
+        <v>58</v>
+      </c>
+      <c r="S33" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T33" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3131,8 +3630,22 @@
       <c r="P34" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q34" t="s">
+        <v>202</v>
+      </c>
+      <c r="R34" t="s">
+        <v>58</v>
+      </c>
+      <c r="S34" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T34" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3182,8 +3695,22 @@
       <c r="P35" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q35" t="s">
+        <v>202</v>
+      </c>
+      <c r="R35" t="s">
+        <v>205</v>
+      </c>
+      <c r="S35" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T35" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3230,8 +3757,22 @@
       <c r="P36" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q36" t="s">
+        <v>202</v>
+      </c>
+      <c r="R36" t="s">
+        <v>205</v>
+      </c>
+      <c r="S36" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T36" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3278,8 +3819,22 @@
       <c r="P37" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q37" t="s">
+        <v>202</v>
+      </c>
+      <c r="R37" t="s">
+        <v>205</v>
+      </c>
+      <c r="S37" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T37" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3326,8 +3881,22 @@
       <c r="P38" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q38" t="s">
+        <v>202</v>
+      </c>
+      <c r="R38" t="s">
+        <v>205</v>
+      </c>
+      <c r="S38" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T38" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3374,8 +3943,22 @@
       <c r="P39" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q39" t="s">
+        <v>206</v>
+      </c>
+      <c r="R39" t="s">
+        <v>109</v>
+      </c>
+      <c r="S39" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T39" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3422,8 +4005,22 @@
       <c r="P40" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q40" t="s">
+        <v>206</v>
+      </c>
+      <c r="R40" t="s">
+        <v>214</v>
+      </c>
+      <c r="S40" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T40" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3470,8 +4067,22 @@
       <c r="P41" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q41" t="s">
+        <v>206</v>
+      </c>
+      <c r="R41" t="s">
+        <v>214</v>
+      </c>
+      <c r="S41" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T41" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3518,8 +4129,22 @@
       <c r="P42" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q42" t="s">
+        <v>206</v>
+      </c>
+      <c r="R42" t="s">
+        <v>214</v>
+      </c>
+      <c r="S42" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T42" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3566,8 +4191,22 @@
       <c r="P43" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q43" t="s">
+        <v>206</v>
+      </c>
+      <c r="R43" t="s">
+        <v>214</v>
+      </c>
+      <c r="S43" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T43" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3614,8 +4253,22 @@
       <c r="P44" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q44" t="s">
+        <v>206</v>
+      </c>
+      <c r="R44" t="s">
+        <v>216</v>
+      </c>
+      <c r="S44" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T44" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3662,8 +4315,22 @@
       <c r="P45" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q45" t="s">
+        <v>206</v>
+      </c>
+      <c r="R45" t="s">
+        <v>216</v>
+      </c>
+      <c r="S45" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T45" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3710,8 +4377,22 @@
       <c r="P46" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q46" t="s">
+        <v>206</v>
+      </c>
+      <c r="R46" t="s">
+        <v>101</v>
+      </c>
+      <c r="S46" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T46" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3758,8 +4439,22 @@
       <c r="P47" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q47" t="s">
+        <v>206</v>
+      </c>
+      <c r="R47" t="s">
+        <v>101</v>
+      </c>
+      <c r="S47" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T47" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3806,8 +4501,22 @@
       <c r="P48" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q48" t="s">
+        <v>206</v>
+      </c>
+      <c r="R48" t="s">
+        <v>101</v>
+      </c>
+      <c r="S48" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T48" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3854,8 +4563,22 @@
       <c r="P49" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q49" t="s">
+        <v>206</v>
+      </c>
+      <c r="R49" t="s">
+        <v>215</v>
+      </c>
+      <c r="S49" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T49" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3902,8 +4625,22 @@
       <c r="P50" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q50" t="s">
+        <v>206</v>
+      </c>
+      <c r="R50" t="s">
+        <v>73</v>
+      </c>
+      <c r="S50" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T50" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3953,8 +4690,22 @@
       <c r="P51" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q51" t="s">
+        <v>206</v>
+      </c>
+      <c r="R51" t="s">
+        <v>116</v>
+      </c>
+      <c r="S51" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T51" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4001,8 +4752,22 @@
       <c r="P52" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q52" t="s">
+        <v>206</v>
+      </c>
+      <c r="R52" t="s">
+        <v>116</v>
+      </c>
+      <c r="S52" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T52" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4049,8 +4814,22 @@
       <c r="P53" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q53" t="s">
+        <v>206</v>
+      </c>
+      <c r="R53" t="s">
+        <v>116</v>
+      </c>
+      <c r="S53" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T53" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4100,8 +4879,22 @@
       <c r="P54" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q54" t="s">
+        <v>16</v>
+      </c>
+      <c r="R54" t="s">
+        <v>16</v>
+      </c>
+      <c r="S54" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T54" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4148,8 +4941,22 @@
       <c r="P55" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q55" t="s">
+        <v>206</v>
+      </c>
+      <c r="R55" t="s">
+        <v>114</v>
+      </c>
+      <c r="S55" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T55" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4196,8 +5003,22 @@
       <c r="P56" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q56" t="s">
+        <v>206</v>
+      </c>
+      <c r="R56" t="s">
+        <v>108</v>
+      </c>
+      <c r="S56" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T56" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4247,8 +5068,22 @@
       <c r="P57" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q57" t="s">
+        <v>16</v>
+      </c>
+      <c r="R57" t="s">
+        <v>16</v>
+      </c>
+      <c r="S57" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T57" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4298,8 +5133,22 @@
       <c r="P58" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q58" t="s">
+        <v>150</v>
+      </c>
+      <c r="R58" t="s">
+        <v>162</v>
+      </c>
+      <c r="S58" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T58" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4346,8 +5195,22 @@
       <c r="P59" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q59" t="s">
+        <v>150</v>
+      </c>
+      <c r="R59" t="s">
+        <v>70</v>
+      </c>
+      <c r="S59" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T59" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4394,8 +5257,22 @@
       <c r="P60" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q60" t="s">
+        <v>150</v>
+      </c>
+      <c r="R60" t="s">
+        <v>11</v>
+      </c>
+      <c r="S60" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T60" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4442,8 +5319,22 @@
       <c r="P61" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q61" t="s">
+        <v>150</v>
+      </c>
+      <c r="R61" t="s">
+        <v>11</v>
+      </c>
+      <c r="S61" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T61" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4490,8 +5381,22 @@
       <c r="P62" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q62" t="s">
+        <v>150</v>
+      </c>
+      <c r="R62" t="s">
+        <v>225</v>
+      </c>
+      <c r="S62" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T62" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4538,8 +5443,22 @@
       <c r="P63" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q63" t="s">
+        <v>150</v>
+      </c>
+      <c r="R63" t="s">
+        <v>203</v>
+      </c>
+      <c r="S63" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T63" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4586,8 +5505,22 @@
       <c r="P64" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q64" t="s">
+        <v>150</v>
+      </c>
+      <c r="R64" t="s">
+        <v>203</v>
+      </c>
+      <c r="S64" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T64" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4637,8 +5570,22 @@
       <c r="P65" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q65" t="s">
+        <v>150</v>
+      </c>
+      <c r="R65" t="s">
+        <v>173</v>
+      </c>
+      <c r="S65" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T65" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4685,8 +5632,22 @@
       <c r="P66" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q66" t="s">
+        <v>150</v>
+      </c>
+      <c r="R66" t="s">
+        <v>72</v>
+      </c>
+      <c r="S66" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="T66" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4718,7 +5679,7 @@
         <v>0</v>
       </c>
       <c r="L67" t="str">
-        <f t="shared" ref="L67:L130" si="1">F67</f>
+        <f t="shared" ref="L67:L130" si="3">F67</f>
         <v>Mambilima</v>
       </c>
       <c r="M67" t="s">
@@ -4733,8 +5694,22 @@
       <c r="P67" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q67" t="s">
+        <v>150</v>
+      </c>
+      <c r="R67" t="s">
+        <v>69</v>
+      </c>
+      <c r="S67" t="b">
+        <f t="shared" ref="S67:S130" si="4">Q67=B67</f>
+        <v>1</v>
+      </c>
+      <c r="T67" t="b">
+        <f t="shared" ref="T67:T130" si="5">Q67=N67</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4766,7 +5741,7 @@
         <v>0</v>
       </c>
       <c r="L68" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Mwense</v>
       </c>
       <c r="M68" t="s">
@@ -4781,8 +5756,22 @@
       <c r="P68" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q68" t="s">
+        <v>150</v>
+      </c>
+      <c r="R68" t="s">
+        <v>69</v>
+      </c>
+      <c r="S68" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T68" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4814,7 +5803,7 @@
         <v>0</v>
       </c>
       <c r="L69" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Nchelenge</v>
       </c>
       <c r="M69" t="s">
@@ -4829,8 +5818,22 @@
       <c r="P69" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q69" t="s">
+        <v>150</v>
+      </c>
+      <c r="R69" t="s">
+        <v>75</v>
+      </c>
+      <c r="S69" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T69" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4862,7 +5865,7 @@
         <v>0</v>
       </c>
       <c r="L70" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Bangweulu</v>
       </c>
       <c r="M70" t="s">
@@ -4877,8 +5880,22 @@
       <c r="P70" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q70" t="s">
+        <v>150</v>
+      </c>
+      <c r="R70" t="s">
+        <v>190</v>
+      </c>
+      <c r="S70" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T70" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4910,7 +5927,7 @@
         <v>0</v>
       </c>
       <c r="L71" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Chifunabuli</v>
       </c>
       <c r="M71" t="s">
@@ -4925,8 +5942,22 @@
       <c r="P71" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q71" t="s">
+        <v>150</v>
+      </c>
+      <c r="R71" t="s">
+        <v>190</v>
+      </c>
+      <c r="S71" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T71" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4958,7 +5989,7 @@
         <v>0</v>
       </c>
       <c r="L72" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Chilanga</v>
       </c>
       <c r="M72" t="s">
@@ -4973,8 +6004,22 @@
       <c r="P72" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q72" t="s">
+        <v>220</v>
+      </c>
+      <c r="R72" t="s">
+        <v>135</v>
+      </c>
+      <c r="S72" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T72" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -5009,7 +6054,7 @@
         <v>0</v>
       </c>
       <c r="L73" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>NA</v>
       </c>
       <c r="M73" t="s">
@@ -5024,8 +6069,22 @@
       <c r="P73" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q73" t="s">
+        <v>16</v>
+      </c>
+      <c r="R73" t="s">
+        <v>16</v>
+      </c>
+      <c r="S73" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T73" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -5057,7 +6116,7 @@
         <v>0</v>
       </c>
       <c r="L74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Chongwe</v>
       </c>
       <c r="M74" t="s">
@@ -5072,8 +6131,22 @@
       <c r="P74" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q74" t="s">
+        <v>220</v>
+      </c>
+      <c r="R74" t="s">
+        <v>134</v>
+      </c>
+      <c r="S74" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T74" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -5105,7 +6178,7 @@
         <v>0</v>
       </c>
       <c r="L75" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Kafue</v>
       </c>
       <c r="M75" t="s">
@@ -5120,8 +6193,22 @@
       <c r="P75" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q75" t="s">
+        <v>220</v>
+      </c>
+      <c r="R75" t="s">
+        <v>128</v>
+      </c>
+      <c r="S75" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T75" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -5153,7 +6240,7 @@
         <v>0</v>
       </c>
       <c r="L76" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Feira</v>
       </c>
       <c r="M76" t="s">
@@ -5168,8 +6255,22 @@
       <c r="P76" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q76" t="s">
+        <v>220</v>
+      </c>
+      <c r="R76" t="s">
+        <v>223</v>
+      </c>
+      <c r="S76" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T76" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -5201,7 +6302,7 @@
         <v>0</v>
       </c>
       <c r="L77" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Chawama</v>
       </c>
       <c r="M77" t="s">
@@ -5216,8 +6317,22 @@
       <c r="P77" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q77" t="s">
+        <v>220</v>
+      </c>
+      <c r="R77" t="s">
+        <v>220</v>
+      </c>
+      <c r="S77" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T77" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -5249,7 +6364,7 @@
         <v>0</v>
       </c>
       <c r="L78" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Kabwata</v>
       </c>
       <c r="M78" t="s">
@@ -5264,8 +6379,22 @@
       <c r="P78" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q78" t="s">
+        <v>220</v>
+      </c>
+      <c r="R78" t="s">
+        <v>220</v>
+      </c>
+      <c r="S78" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T78" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5297,7 +6426,7 @@
         <v>0</v>
       </c>
       <c r="L79" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Kanyama</v>
       </c>
       <c r="M79" t="s">
@@ -5312,8 +6441,22 @@
       <c r="P79" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q79" t="s">
+        <v>220</v>
+      </c>
+      <c r="R79" t="s">
+        <v>220</v>
+      </c>
+      <c r="S79" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T79" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5345,7 +6488,7 @@
         <v>0</v>
       </c>
       <c r="L80" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Lusaka Central</v>
       </c>
       <c r="M80" t="s">
@@ -5360,8 +6503,22 @@
       <c r="P80" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q80" t="s">
+        <v>220</v>
+      </c>
+      <c r="R80" t="s">
+        <v>220</v>
+      </c>
+      <c r="S80" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T80" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5393,7 +6550,7 @@
         <v>0</v>
       </c>
       <c r="L81" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Mandevu</v>
       </c>
       <c r="M81" t="s">
@@ -5408,8 +6565,22 @@
       <c r="P81" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q81" t="s">
+        <v>220</v>
+      </c>
+      <c r="R81" t="s">
+        <v>220</v>
+      </c>
+      <c r="S81" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T81" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5441,7 +6612,7 @@
         <v>0</v>
       </c>
       <c r="L82" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Matero</v>
       </c>
       <c r="M82" t="s">
@@ -5456,8 +6627,22 @@
       <c r="P82" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q82" t="s">
+        <v>220</v>
+      </c>
+      <c r="R82" t="s">
+        <v>220</v>
+      </c>
+      <c r="S82" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T82" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5489,7 +6674,7 @@
         <v>0</v>
       </c>
       <c r="L83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Munali</v>
       </c>
       <c r="M83" t="s">
@@ -5504,8 +6689,22 @@
       <c r="P83" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q83" t="s">
+        <v>220</v>
+      </c>
+      <c r="R83" t="s">
+        <v>220</v>
+      </c>
+      <c r="S83" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T83" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5537,7 +6736,7 @@
         <v>0</v>
       </c>
       <c r="L84" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Rufunsa</v>
       </c>
       <c r="M84" t="s">
@@ -5552,8 +6751,22 @@
       <c r="P84" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q84" t="s">
+        <v>220</v>
+      </c>
+      <c r="R84" t="s">
+        <v>133</v>
+      </c>
+      <c r="S84" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T84" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5585,7 +6798,7 @@
         <v>0</v>
       </c>
       <c r="L85" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Mwembezhi</v>
       </c>
       <c r="M85" t="s">
@@ -5600,8 +6813,22 @@
       <c r="P85" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q85" t="s">
+        <v>220</v>
+      </c>
+      <c r="R85" t="s">
+        <v>221</v>
+      </c>
+      <c r="S85" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T85" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5633,7 +6860,7 @@
         <v>0</v>
       </c>
       <c r="L86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Chama North</v>
       </c>
       <c r="M86" t="s">
@@ -5648,8 +6875,22 @@
       <c r="P86" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q86" t="s">
+        <v>119</v>
+      </c>
+      <c r="R86" t="s">
+        <v>213</v>
+      </c>
+      <c r="S86" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T86" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5681,7 +6922,7 @@
         <v>0</v>
       </c>
       <c r="L87" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Chama South</v>
       </c>
       <c r="M87" t="s">
@@ -5696,8 +6937,22 @@
       <c r="P87" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q87" t="s">
+        <v>119</v>
+      </c>
+      <c r="R87" t="s">
+        <v>213</v>
+      </c>
+      <c r="S87" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T87" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5729,7 +6984,7 @@
         <v>0</v>
       </c>
       <c r="L88" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Chinsali</v>
       </c>
       <c r="M88" t="s">
@@ -5744,8 +6999,22 @@
       <c r="P88" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q88" t="s">
+        <v>119</v>
+      </c>
+      <c r="R88" t="s">
+        <v>89</v>
+      </c>
+      <c r="S88" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T88" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5780,7 +7049,7 @@
         <v>5</v>
       </c>
       <c r="L89" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Isoka</v>
       </c>
       <c r="M89" t="s">
@@ -5795,8 +7064,22 @@
       <c r="P89" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q89" t="s">
+        <v>119</v>
+      </c>
+      <c r="R89" t="s">
+        <v>164</v>
+      </c>
+      <c r="S89" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T89" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5831,7 +7114,7 @@
         <v>280</v>
       </c>
       <c r="L90" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Mafinga</v>
       </c>
       <c r="M90" t="s">
@@ -5846,8 +7129,22 @@
       <c r="P90" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q90" t="s">
+        <v>119</v>
+      </c>
+      <c r="R90" t="s">
+        <v>166</v>
+      </c>
+      <c r="S90" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T90" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5879,7 +7176,7 @@
         <v>0</v>
       </c>
       <c r="L91" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Kanchibiya</v>
       </c>
       <c r="M91" t="s">
@@ -5894,8 +7191,22 @@
       <c r="P91" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q91" t="s">
+        <v>119</v>
+      </c>
+      <c r="R91" t="s">
+        <v>167</v>
+      </c>
+      <c r="S91" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T91" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5927,7 +7238,7 @@
         <v>0</v>
       </c>
       <c r="L92" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Mfuwe</v>
       </c>
       <c r="M92" t="s">
@@ -5942,8 +7253,22 @@
       <c r="P92" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q92" t="s">
+        <v>119</v>
+      </c>
+      <c r="R92" t="s">
+        <v>167</v>
+      </c>
+      <c r="S92" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T92" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5978,7 +7303,7 @@
         <v>5</v>
       </c>
       <c r="L93" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Mpika</v>
       </c>
       <c r="M93" t="s">
@@ -5993,8 +7318,22 @@
       <c r="P93" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q93" t="s">
+        <v>119</v>
+      </c>
+      <c r="R93" t="s">
+        <v>167</v>
+      </c>
+      <c r="S93" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T93" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6026,7 +7365,7 @@
         <v>0</v>
       </c>
       <c r="L94" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Nakonde</v>
       </c>
       <c r="M94" t="s">
@@ -6041,8 +7380,22 @@
       <c r="P94" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q94" t="s">
+        <v>119</v>
+      </c>
+      <c r="R94" t="s">
+        <v>78</v>
+      </c>
+      <c r="S94" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T94" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -6091,8 +7444,22 @@
       <c r="P95" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q95" t="s">
+        <v>119</v>
+      </c>
+      <c r="R95" t="s">
+        <v>172</v>
+      </c>
+      <c r="S95" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T95" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6124,7 +7491,7 @@
         <v>0</v>
       </c>
       <c r="L96" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Chavuma</v>
       </c>
       <c r="M96" t="s">
@@ -6139,8 +7506,22 @@
       <c r="P96" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q96" t="s">
+        <v>199</v>
+      </c>
+      <c r="R96" t="s">
+        <v>33</v>
+      </c>
+      <c r="S96" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T96" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -6175,7 +7556,7 @@
         <v>281</v>
       </c>
       <c r="L97" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Ikeleng'i</v>
       </c>
       <c r="M97" t="s">
@@ -6190,8 +7571,22 @@
       <c r="P97" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q97" t="s">
+        <v>199</v>
+      </c>
+      <c r="R97" t="s">
+        <v>174</v>
+      </c>
+      <c r="S97" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T97" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6226,7 +7621,7 @@
         <v>280</v>
       </c>
       <c r="L98" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Kabompo West</v>
       </c>
       <c r="M98" t="s">
@@ -6241,8 +7636,22 @@
       <c r="P98" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q98" t="s">
+        <v>199</v>
+      </c>
+      <c r="R98" t="s">
+        <v>184</v>
+      </c>
+      <c r="S98" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T98" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -6274,7 +7683,7 @@
         <v>0</v>
       </c>
       <c r="L99" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Kasempa</v>
       </c>
       <c r="M99" t="s">
@@ -6289,8 +7698,22 @@
       <c r="P99" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q99" t="s">
+        <v>199</v>
+      </c>
+      <c r="R99" t="s">
+        <v>40</v>
+      </c>
+      <c r="S99" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T99" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -6325,7 +7748,7 @@
         <v>280</v>
       </c>
       <c r="L100" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Kabompo East</v>
       </c>
       <c r="M100" t="s">
@@ -6340,8 +7763,22 @@
       <c r="P100" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q100" t="s">
+        <v>199</v>
+      </c>
+      <c r="R100" t="s">
+        <v>185</v>
+      </c>
+      <c r="S100" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T100" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -6373,7 +7810,7 @@
         <v>0</v>
       </c>
       <c r="L101" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Mufumbwe</v>
       </c>
       <c r="M101" t="s">
@@ -6388,8 +7825,22 @@
       <c r="P101" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q101" t="s">
+        <v>199</v>
+      </c>
+      <c r="R101" t="s">
+        <v>39</v>
+      </c>
+      <c r="S101" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T101" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -6424,7 +7875,7 @@
         <v>5</v>
       </c>
       <c r="L102" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Mwinilunga</v>
       </c>
       <c r="M102" t="s">
@@ -6439,8 +7890,22 @@
       <c r="P102" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q102" t="s">
+        <v>199</v>
+      </c>
+      <c r="R102" t="s">
+        <v>168</v>
+      </c>
+      <c r="S102" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T102" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -6472,7 +7937,7 @@
         <v>0</v>
       </c>
       <c r="L103" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Solwezi Central</v>
       </c>
       <c r="M103" t="s">
@@ -6487,8 +7952,22 @@
       <c r="P103" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q103" t="s">
+        <v>199</v>
+      </c>
+      <c r="R103" t="s">
+        <v>201</v>
+      </c>
+      <c r="S103" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T103" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -6520,7 +7999,7 @@
         <v>0</v>
       </c>
       <c r="L104" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Solwezi East</v>
       </c>
       <c r="M104" t="s">
@@ -6535,8 +8014,22 @@
       <c r="P104" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q104" t="s">
+        <v>199</v>
+      </c>
+      <c r="R104" t="s">
+        <v>201</v>
+      </c>
+      <c r="S104" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T104" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -6568,7 +8061,7 @@
         <v>0</v>
       </c>
       <c r="L105" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Solwezi West</v>
       </c>
       <c r="M105" t="s">
@@ -6583,8 +8076,22 @@
       <c r="P105" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q105" t="s">
+        <v>199</v>
+      </c>
+      <c r="R105" t="s">
+        <v>201</v>
+      </c>
+      <c r="S105" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T105" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -6616,7 +8123,7 @@
         <v>0</v>
       </c>
       <c r="L106" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Zambezi East</v>
       </c>
       <c r="M106" t="s">
@@ -6631,8 +8138,22 @@
       <c r="P106" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q106" t="s">
+        <v>199</v>
+      </c>
+      <c r="R106" t="s">
+        <v>200</v>
+      </c>
+      <c r="S106" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T106" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -6664,7 +8185,7 @@
         <v>0</v>
       </c>
       <c r="L107" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Zambezi West</v>
       </c>
       <c r="M107" t="s">
@@ -6679,8 +8200,22 @@
       <c r="P107" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q107" t="s">
+        <v>199</v>
+      </c>
+      <c r="R107" t="s">
+        <v>200</v>
+      </c>
+      <c r="S107" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T107" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -6712,7 +8247,7 @@
         <v>0</v>
       </c>
       <c r="L108" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Chilubi</v>
       </c>
       <c r="M108" t="s">
@@ -6727,8 +8262,22 @@
       <c r="P108" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q108" t="s">
+        <v>207</v>
+      </c>
+      <c r="R108" t="s">
+        <v>91</v>
+      </c>
+      <c r="S108" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T108" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -6760,7 +8309,7 @@
         <v>0</v>
       </c>
       <c r="L109" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Kaputa</v>
       </c>
       <c r="M109" t="s">
@@ -6775,8 +8324,22 @@
       <c r="P109" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q109" t="s">
+        <v>207</v>
+      </c>
+      <c r="R109" t="s">
+        <v>81</v>
+      </c>
+      <c r="S109" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T109" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -6808,7 +8371,7 @@
         <v>0</v>
       </c>
       <c r="L110" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Kasama Central</v>
       </c>
       <c r="M110" t="s">
@@ -6823,8 +8386,22 @@
       <c r="P110" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q110" t="s">
+        <v>207</v>
+      </c>
+      <c r="R110" t="s">
+        <v>211</v>
+      </c>
+      <c r="S110" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T110" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -6856,7 +8433,7 @@
         <v>0</v>
       </c>
       <c r="L111" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Lukashya</v>
       </c>
       <c r="M111" t="s">
@@ -6871,8 +8448,22 @@
       <c r="P111" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q111" t="s">
+        <v>207</v>
+      </c>
+      <c r="R111" t="s">
+        <v>211</v>
+      </c>
+      <c r="S111" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T111" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -6904,7 +8495,7 @@
         <v>0</v>
       </c>
       <c r="L112" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Lubansenshi</v>
       </c>
       <c r="M112" t="s">
@@ -6919,8 +8510,22 @@
       <c r="P112" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q112" t="s">
+        <v>207</v>
+      </c>
+      <c r="R112" t="s">
+        <v>209</v>
+      </c>
+      <c r="S112" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T112" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -6952,7 +8557,7 @@
         <v>0</v>
       </c>
       <c r="L113" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Lupososhi</v>
       </c>
       <c r="M113" t="s">
@@ -6967,8 +8572,22 @@
       <c r="P113" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q113" t="s">
+        <v>207</v>
+      </c>
+      <c r="R113" t="s">
+        <v>209</v>
+      </c>
+      <c r="S113" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T113" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -7000,7 +8619,7 @@
         <v>0</v>
       </c>
       <c r="L114" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Mbala</v>
       </c>
       <c r="M114" t="s">
@@ -7015,8 +8634,22 @@
       <c r="P114" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q114" t="s">
+        <v>207</v>
+      </c>
+      <c r="R114" t="s">
+        <v>79</v>
+      </c>
+      <c r="S114" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T114" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -7048,7 +8681,7 @@
         <v>0</v>
       </c>
       <c r="L115" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Senga Hill</v>
       </c>
       <c r="M115" t="s">
@@ -7063,8 +8696,22 @@
       <c r="P115" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q115" t="s">
+        <v>207</v>
+      </c>
+      <c r="R115" t="s">
+        <v>79</v>
+      </c>
+      <c r="S115" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T115" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -7096,7 +8743,7 @@
         <v>0</v>
       </c>
       <c r="L116" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Lunte</v>
       </c>
       <c r="M116" t="s">
@@ -7111,8 +8758,22 @@
       <c r="P116" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q116" t="s">
+        <v>207</v>
+      </c>
+      <c r="R116" t="s">
+        <v>83</v>
+      </c>
+      <c r="S116" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T116" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -7144,7 +8805,7 @@
         <v>0</v>
       </c>
       <c r="L117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Mporokoso</v>
       </c>
       <c r="M117" t="s">
@@ -7159,8 +8820,22 @@
       <c r="P117" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q117" t="s">
+        <v>207</v>
+      </c>
+      <c r="R117" t="s">
+        <v>83</v>
+      </c>
+      <c r="S117" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T117" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -7192,7 +8867,7 @@
         <v>0</v>
       </c>
       <c r="L118" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Mpulungu</v>
       </c>
       <c r="M118" t="s">
@@ -7207,8 +8882,22 @@
       <c r="P118" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q118" t="s">
+        <v>207</v>
+      </c>
+      <c r="R118" t="s">
+        <v>80</v>
+      </c>
+      <c r="S118" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T118" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -7240,7 +8929,7 @@
         <v>0</v>
       </c>
       <c r="L119" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Malole</v>
       </c>
       <c r="M119" t="s">
@@ -7255,8 +8944,22 @@
       <c r="P119" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q119" t="s">
+        <v>207</v>
+      </c>
+      <c r="R119" t="s">
+        <v>210</v>
+      </c>
+      <c r="S119" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T119" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -7288,7 +8991,7 @@
         <v>0</v>
       </c>
       <c r="L120" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Chimbamilonga</v>
       </c>
       <c r="M120" t="s">
@@ -7303,8 +9006,22 @@
       <c r="P120" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q120" t="s">
+        <v>207</v>
+      </c>
+      <c r="R120" t="s">
+        <v>208</v>
+      </c>
+      <c r="S120" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T120" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -7336,7 +9053,7 @@
         <v>0</v>
       </c>
       <c r="L121" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Chikankata</v>
       </c>
       <c r="M121" t="s">
@@ -7351,8 +9068,22 @@
       <c r="P121" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q121" t="s">
+        <v>191</v>
+      </c>
+      <c r="R121" t="s">
+        <v>146</v>
+      </c>
+      <c r="S121" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T121" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -7384,7 +9115,7 @@
         <v>0</v>
       </c>
       <c r="L122" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Choma Central</v>
       </c>
       <c r="M122" t="s">
@@ -7399,8 +9130,22 @@
       <c r="P122" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q122" t="s">
+        <v>191</v>
+      </c>
+      <c r="R122" t="s">
+        <v>226</v>
+      </c>
+      <c r="S122" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T122" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -7432,7 +9177,7 @@
         <v>0</v>
       </c>
       <c r="L123" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Mbabala</v>
       </c>
       <c r="M123" t="s">
@@ -7447,8 +9192,22 @@
       <c r="P123" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q123" t="s">
+        <v>191</v>
+      </c>
+      <c r="R123" t="s">
+        <v>226</v>
+      </c>
+      <c r="S123" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T123" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -7480,7 +9239,7 @@
         <v>0</v>
       </c>
       <c r="L124" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Gwembe</v>
       </c>
       <c r="M124" t="s">
@@ -7495,8 +9254,22 @@
       <c r="P124" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q124" t="s">
+        <v>191</v>
+      </c>
+      <c r="R124" t="s">
+        <v>145</v>
+      </c>
+      <c r="S124" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T124" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -7528,7 +9301,7 @@
         <v>0</v>
       </c>
       <c r="L125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Dundumwezi</v>
       </c>
       <c r="M125" t="s">
@@ -7543,8 +9316,22 @@
       <c r="P125" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q125" t="s">
+        <v>191</v>
+      </c>
+      <c r="R125" t="s">
+        <v>228</v>
+      </c>
+      <c r="S125" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T125" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -7576,7 +9363,7 @@
         <v>0</v>
       </c>
       <c r="L126" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Kalomo Central</v>
       </c>
       <c r="M126" t="s">
@@ -7591,8 +9378,22 @@
       <c r="P126" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q126" t="s">
+        <v>191</v>
+      </c>
+      <c r="R126" t="s">
+        <v>228</v>
+      </c>
+      <c r="S126" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T126" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -7624,7 +9425,7 @@
         <v>0</v>
       </c>
       <c r="L127" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Katombola</v>
       </c>
       <c r="M127" t="s">
@@ -7639,8 +9440,22 @@
       <c r="P127" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q127" t="s">
+        <v>191</v>
+      </c>
+      <c r="R127" t="s">
+        <v>229</v>
+      </c>
+      <c r="S127" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T127" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -7672,7 +9487,7 @@
         <v>0</v>
       </c>
       <c r="L128" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Livingstone</v>
       </c>
       <c r="M128" t="s">
@@ -7687,8 +9502,22 @@
       <c r="P128" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q128" t="s">
+        <v>191</v>
+      </c>
+      <c r="R128" t="s">
+        <v>157</v>
+      </c>
+      <c r="S128" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T128" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -7720,7 +9549,7 @@
         <v>0</v>
       </c>
       <c r="L129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Magoye</v>
       </c>
       <c r="M129" t="s">
@@ -7735,8 +9564,22 @@
       <c r="P129" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q129" t="s">
+        <v>191</v>
+      </c>
+      <c r="R129" t="s">
+        <v>224</v>
+      </c>
+      <c r="S129" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T129" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -7768,7 +9611,7 @@
         <v>0</v>
       </c>
       <c r="L130" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Mazabuka Central</v>
       </c>
       <c r="M130" t="s">
@@ -7783,8 +9626,22 @@
       <c r="P130" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q130" t="s">
+        <v>191</v>
+      </c>
+      <c r="R130" t="s">
+        <v>224</v>
+      </c>
+      <c r="S130" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T130" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -7816,7 +9673,7 @@
         <v>0</v>
       </c>
       <c r="L131" t="str">
-        <f t="shared" ref="L131:L157" si="2">F131</f>
+        <f t="shared" ref="L131:L157" si="6">F131</f>
         <v>Bweengwa</v>
       </c>
       <c r="M131" t="s">
@@ -7831,8 +9688,22 @@
       <c r="P131" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q131" t="s">
+        <v>191</v>
+      </c>
+      <c r="R131" t="s">
+        <v>192</v>
+      </c>
+      <c r="S131" t="b">
+        <f t="shared" ref="S131:S157" si="7">Q131=B131</f>
+        <v>1</v>
+      </c>
+      <c r="T131" t="b">
+        <f t="shared" ref="T131:T157" si="8">Q131=N131</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -7864,7 +9735,7 @@
         <v>0</v>
       </c>
       <c r="L132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Monze Central</v>
       </c>
       <c r="M132" t="s">
@@ -7879,8 +9750,22 @@
       <c r="P132" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q132" t="s">
+        <v>191</v>
+      </c>
+      <c r="R132" t="s">
+        <v>192</v>
+      </c>
+      <c r="S132" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T132" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -7912,7 +9797,7 @@
         <v>0</v>
       </c>
       <c r="L133" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Moomba</v>
       </c>
       <c r="M133" t="s">
@@ -7927,8 +9812,22 @@
       <c r="P133" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q133" t="s">
+        <v>191</v>
+      </c>
+      <c r="R133" t="s">
+        <v>192</v>
+      </c>
+      <c r="S133" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T133" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -7960,7 +9859,7 @@
         <v>0</v>
       </c>
       <c r="L134" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Namwala</v>
       </c>
       <c r="M134" t="s">
@@ -7975,8 +9874,22 @@
       <c r="P134" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q134" t="s">
+        <v>191</v>
+      </c>
+      <c r="R134" t="s">
+        <v>14</v>
+      </c>
+      <c r="S134" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T134" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -8008,7 +9921,7 @@
         <v>0</v>
       </c>
       <c r="L135" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Pemba</v>
       </c>
       <c r="M135" t="s">
@@ -8023,8 +9936,22 @@
       <c r="P135" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q135" t="s">
+        <v>191</v>
+      </c>
+      <c r="R135" t="s">
+        <v>152</v>
+      </c>
+      <c r="S135" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T135" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -8056,7 +9983,7 @@
         <v>0</v>
       </c>
       <c r="L136" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Siavonga</v>
       </c>
       <c r="M136" t="s">
@@ -8071,8 +9998,22 @@
       <c r="P136" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q136" t="s">
+        <v>191</v>
+      </c>
+      <c r="R136" t="s">
+        <v>144</v>
+      </c>
+      <c r="S136" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T136" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -8104,7 +10045,7 @@
         <v>0</v>
       </c>
       <c r="L137" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Sinazongwe</v>
       </c>
       <c r="M137" t="s">
@@ -8119,8 +10060,22 @@
       <c r="P137" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q137" t="s">
+        <v>191</v>
+      </c>
+      <c r="R137" t="s">
+        <v>153</v>
+      </c>
+      <c r="S137" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T137" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -8152,7 +10107,7 @@
         <v>0</v>
       </c>
       <c r="L138" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Mapatizya</v>
       </c>
       <c r="M138" t="s">
@@ -8167,8 +10122,22 @@
       <c r="P138" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q138" t="s">
+        <v>191</v>
+      </c>
+      <c r="R138" t="s">
+        <v>227</v>
+      </c>
+      <c r="S138" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T138" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -8200,7 +10169,7 @@
         <v>0</v>
       </c>
       <c r="L139" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Kalabo Central</v>
       </c>
       <c r="M139" t="s">
@@ -8215,8 +10184,22 @@
       <c r="P139" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q139" t="s">
+        <v>193</v>
+      </c>
+      <c r="R139" t="s">
+        <v>198</v>
+      </c>
+      <c r="S139" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T139" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -8248,7 +10231,7 @@
         <v>0</v>
       </c>
       <c r="L140" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Liuwa</v>
       </c>
       <c r="M140" t="s">
@@ -8263,8 +10246,22 @@
       <c r="P140" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q140" t="s">
+        <v>193</v>
+      </c>
+      <c r="R140" t="s">
+        <v>198</v>
+      </c>
+      <c r="S140" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T140" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -8296,7 +10293,7 @@
         <v>0</v>
       </c>
       <c r="L141" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Kaoma Central</v>
       </c>
       <c r="M141" t="s">
@@ -8311,8 +10308,22 @@
       <c r="P141" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q141" t="s">
+        <v>193</v>
+      </c>
+      <c r="R141" t="s">
+        <v>194</v>
+      </c>
+      <c r="S141" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T141" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -8344,7 +10355,7 @@
         <v>0</v>
       </c>
       <c r="L142" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Mangango</v>
       </c>
       <c r="M142" t="s">
@@ -8359,8 +10370,22 @@
       <c r="P142" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q142" t="s">
+        <v>193</v>
+      </c>
+      <c r="R142" t="s">
+        <v>194</v>
+      </c>
+      <c r="S142" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T142" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -8392,7 +10417,7 @@
         <v>0</v>
       </c>
       <c r="L143" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Luena</v>
       </c>
       <c r="M143" t="s">
@@ -8407,8 +10432,22 @@
       <c r="P143" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q143" t="s">
+        <v>193</v>
+      </c>
+      <c r="R143" t="s">
+        <v>196</v>
+      </c>
+      <c r="S143" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T143" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -8440,7 +10479,7 @@
         <v>0</v>
       </c>
       <c r="L144" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Luampa</v>
       </c>
       <c r="M144" t="s">
@@ -8455,8 +10494,22 @@
       <c r="P144" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q144" t="s">
+        <v>193</v>
+      </c>
+      <c r="R144" t="s">
+        <v>22</v>
+      </c>
+      <c r="S144" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T144" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -8488,7 +10541,7 @@
         <v>0</v>
       </c>
       <c r="L145" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Lukulu East</v>
       </c>
       <c r="M145" t="s">
@@ -8503,8 +10556,22 @@
       <c r="P145" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q145" t="s">
+        <v>193</v>
+      </c>
+      <c r="R145" t="s">
+        <v>197</v>
+      </c>
+      <c r="S145" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T145" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -8539,7 +10606,7 @@
         <v>280</v>
       </c>
       <c r="L146" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Lukulu West</v>
       </c>
       <c r="M146" t="s">
@@ -8554,8 +10621,22 @@
       <c r="P146" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q146" t="s">
+        <v>193</v>
+      </c>
+      <c r="R146" t="s">
+        <v>186</v>
+      </c>
+      <c r="S146" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T146" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -8587,7 +10668,7 @@
         <v>0</v>
       </c>
       <c r="L147" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Mongu Central</v>
       </c>
       <c r="M147" t="s">
@@ -8602,8 +10683,22 @@
       <c r="P147" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q147" t="s">
+        <v>193</v>
+      </c>
+      <c r="R147" t="s">
+        <v>195</v>
+      </c>
+      <c r="S147" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T147" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -8635,7 +10730,7 @@
         <v>0</v>
       </c>
       <c r="L148" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Nalikwanda</v>
       </c>
       <c r="M148" t="s">
@@ -8650,8 +10745,22 @@
       <c r="P148" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q148" t="s">
+        <v>193</v>
+      </c>
+      <c r="R148" t="s">
+        <v>195</v>
+      </c>
+      <c r="S148" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T148" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -8683,7 +10792,7 @@
         <v>0</v>
       </c>
       <c r="L149" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Mulobezi</v>
       </c>
       <c r="M149" t="s">
@@ -8698,8 +10807,22 @@
       <c r="P149" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q149" t="s">
+        <v>193</v>
+      </c>
+      <c r="R149" t="s">
+        <v>18</v>
+      </c>
+      <c r="S149" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T149" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -8731,7 +10854,7 @@
         <v>0</v>
       </c>
       <c r="L150" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Mwandi</v>
       </c>
       <c r="M150" t="s">
@@ -8746,8 +10869,22 @@
       <c r="P150" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q150" t="s">
+        <v>193</v>
+      </c>
+      <c r="R150" t="s">
+        <v>17</v>
+      </c>
+      <c r="S150" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T150" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -8779,7 +10916,7 @@
         <v>0</v>
       </c>
       <c r="L151" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Nalolo</v>
       </c>
       <c r="M151" t="s">
@@ -8794,8 +10931,22 @@
       <c r="P151" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q151" t="s">
+        <v>193</v>
+      </c>
+      <c r="R151" t="s">
+        <v>21</v>
+      </c>
+      <c r="S151" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T151" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -8830,7 +10981,7 @@
         <v>0</v>
       </c>
       <c r="L152" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>NA</v>
       </c>
       <c r="M152" t="s">
@@ -8845,8 +10996,22 @@
       <c r="P152" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q152" t="s">
+        <v>16</v>
+      </c>
+      <c r="R152" t="s">
+        <v>16</v>
+      </c>
+      <c r="S152" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T152" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -8881,7 +11046,7 @@
         <v>5</v>
       </c>
       <c r="L153" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Senanga</v>
       </c>
       <c r="M153" t="s">
@@ -8896,8 +11061,22 @@
       <c r="P153" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q153" t="s">
+        <v>193</v>
+      </c>
+      <c r="R153" t="s">
+        <v>169</v>
+      </c>
+      <c r="S153" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T153" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -8932,7 +11111,7 @@
         <v>5</v>
       </c>
       <c r="L154" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Sesheke</v>
       </c>
       <c r="M154" t="s">
@@ -8947,8 +11126,22 @@
       <c r="P154" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q154" t="s">
+        <v>193</v>
+      </c>
+      <c r="R154" t="s">
+        <v>171</v>
+      </c>
+      <c r="S154" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T154" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -8983,7 +11176,7 @@
         <v>280</v>
       </c>
       <c r="L155" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Sinjembela</v>
       </c>
       <c r="M155" t="s">
@@ -8998,8 +11191,22 @@
       <c r="P155" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q155" t="s">
+        <v>193</v>
+      </c>
+      <c r="R155" t="s">
+        <v>187</v>
+      </c>
+      <c r="S155" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T155" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
@@ -9031,7 +11238,7 @@
         <v>0</v>
       </c>
       <c r="L156" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Sikongo</v>
       </c>
       <c r="M156" t="s">
@@ -9046,8 +11253,22 @@
       <c r="P156" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q156" t="s">
+        <v>193</v>
+      </c>
+      <c r="R156" t="s">
+        <v>117</v>
+      </c>
+      <c r="S156" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T156" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -9082,7 +11303,7 @@
         <v>0</v>
       </c>
       <c r="L157" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>NA</v>
       </c>
       <c r="M157" t="s">
@@ -9097,8 +11318,22 @@
       <c r="P157" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q157" t="s">
+        <v>16</v>
+      </c>
+      <c r="R157" t="s">
+        <v>16</v>
+      </c>
+      <c r="S157" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T157" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
       <c r="D158" s="2"/>
@@ -9108,7 +11343,7 @@
       <c r="H158" s="2"/>
       <c r="I158" s="2"/>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
       <c r="D159" s="2"/>
@@ -9118,7 +11353,7 @@
       <c r="H159" s="2"/>
       <c r="I159" s="2"/>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
       <c r="D160" s="2"/>
@@ -17337,7 +19572,7 @@
         <v>1</v>
       </c>
       <c r="T131" t="str">
-        <f t="shared" ref="T131:T177" si="5">IF(R131=TRUE, P131,S131)</f>
+        <f t="shared" ref="T131:T156" si="5">IF(R131=TRUE, P131,S131)</f>
         <v>Bweengwa</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates on when province shift happened
</commit_message>
<xml_diff>
--- a/ZMB_admin_crosswalk.xlsx
+++ b/ZMB_admin_crosswalk.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="640" windowWidth="28160" windowHeight="15760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="640" windowWidth="28160" windowHeight="15760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="number of constituencies" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8217" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8218" uniqueCount="313">
   <si>
     <t>provinces</t>
   </si>
@@ -972,6 +972,9 @@
   <si>
     <t>Added Muchinga province</t>
   </si>
+  <si>
+    <t>72 districts till 2013 according to Tessam</t>
+  </si>
 </sst>
 </file>
 
@@ -1371,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1442,22 +1445,40 @@
       <c r="E4" t="s">
         <v>286</v>
       </c>
+      <c r="F4" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2011</v>
       </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>72</v>
+      </c>
       <c r="D5">
         <v>150</v>
       </c>
       <c r="E5">
         <v>1421</v>
+      </c>
+      <c r="F5" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2008</v>
       </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>72</v>
+      </c>
       <c r="D6">
         <v>150</v>
       </c>
@@ -1470,13 +1491,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D7">
         <v>150</v>
-      </c>
-      <c r="F7" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1509,7 +1527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q1" sqref="Q1"/>
     </sheetView>

</xml_diff>